<commit_message>
developing LIDAR correlation test code
</commit_message>
<xml_diff>
--- a/docs/LIDAR/Rain Simulation (cross correlation).xlsx
+++ b/docs/LIDAR/Rain Simulation (cross correlation).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnp\Dropbox\Programming\c++\LIDAR\docs\LIDAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB61C46-9153-4222-8CCD-6BD44A52731E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85267E87-777B-47CD-89CC-D14F68928733}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{6F829C6E-AC9C-4B9E-9DA9-8841D05EEE17}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Car</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>Max Corr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Noise </t>
+  </si>
+  <si>
+    <t>Starting to miss</t>
   </si>
 </sst>
 </file>
@@ -628,7 +634,496 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Car Signal + Rain Noise=250</a:t>
+              <a:t>Maximum Correlation</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> v Noise</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$X$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Max Corr</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$W$5:$W$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>350</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$X$5:$X$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5B29-431E-86BB-6BFE505C6E5A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1483921472"/>
+        <c:axId val="1483916896"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1483921472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Rain Noise Factor</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1483916896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1483916896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.60000000000000009"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Maximum Correlation</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1483921472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>No Car Signal + Rain Noise=350</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -928,217 +1423,217 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="71"/>
                 <c:pt idx="0">
-                  <c:v>0.69560557341907825</c:v>
+                  <c:v>6.8214804063860754E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.47481243301178988</c:v>
+                  <c:v>0.69085631349782284</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.65916398713826374</c:v>
+                  <c:v>0.62699564586357037</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.962486602357985</c:v>
+                  <c:v>0.13207547169811321</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.43086816720257232</c:v>
+                  <c:v>0.43976777939042078</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.46409431939978563</c:v>
+                  <c:v>0.69521044992743108</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.88210075026795287</c:v>
+                  <c:v>0.58345428156748924</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.40192926045016075</c:v>
+                  <c:v>0.26124818577648773</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.36763129689174701</c:v>
+                  <c:v>5.3701015965166916E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.91425509110396563</c:v>
+                  <c:v>0.50943396226415083</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.97749196141479089</c:v>
+                  <c:v>0.62264150943396235</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.54126473740621661</c:v>
+                  <c:v>0.59651669085631365</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.89710610932475876</c:v>
+                  <c:v>0.25399129172714074</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.67202572347266876</c:v>
+                  <c:v>0.89550072568940486</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.55412647374062163</c:v>
+                  <c:v>0.44267053701015974</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.5787781350482315</c:v>
+                  <c:v>0.57184325108853395</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.56698821007502687</c:v>
+                  <c:v>0.87808417997097243</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.729903536977492</c:v>
+                  <c:v>0.76197387518142223</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.91318327974276536</c:v>
+                  <c:v>0.59216255442670529</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.66988210075026799</c:v>
+                  <c:v>0.79535558780841797</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.52411575562700974</c:v>
+                  <c:v>0.37880986937590727</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.46516613076098606</c:v>
+                  <c:v>0.37010159651669094</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.9163987138263664</c:v>
+                  <c:v>0.6371552975326561</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.92282958199356924</c:v>
+                  <c:v>0.42089985486211901</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.60450160771704187</c:v>
+                  <c:v>0.65892597968069677</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.7513397642015005</c:v>
+                  <c:v>0.34833091436865021</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.48874598070739556</c:v>
+                  <c:v>0.81132075471698128</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.82422293676312963</c:v>
+                  <c:v>0.92597968069666181</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.59056806002143625</c:v>
+                  <c:v>0.93759071117561665</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.45659163987138263</c:v>
+                  <c:v>0.98258345428156757</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.40407288317256157</c:v>
+                  <c:v>0.5341074020319303</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.47481243301178988</c:v>
+                  <c:v>0.97677793904208998</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.57556270096463014</c:v>
+                  <c:v>0.30624092888243848</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.59485530546623799</c:v>
+                  <c:v>0.45718432510885343</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.69774919614147912</c:v>
+                  <c:v>0.85195936139332351</c:v>
                 </c:pt>
                 <c:pt idx="35">
+                  <c:v>0.63860667634252544</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.42670537010159643</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.9158200290275762</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.45718432510885343</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.4513788098693836E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.81857764876632799</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.52539912917271414</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.45137880986937606</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.26415094339622641</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.83599419448476042</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.33236574746008718</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.47460087082728608</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.89550072568940486</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.94339622641509424</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.64005805515239478</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.29898403483309149</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.74020319303338156</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.4412191582002904</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.74600870827285926</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.85050798258345439</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.17271407837445565</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.15965166908563128</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.29753265602322215</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.77793904208998554</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.99129172714078362</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.87663280116110309</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.55007256894049361</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.38751814223512332</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.98548621190130625</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.75761973875181421</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>9.5791001451378824E-2</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.51814223512336721</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.1204644412191582</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.63280116110304807</c:v>
+                </c:pt>
+                <c:pt idx="70">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.1843515541264738</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.56806002143622714</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0.30225080385852093</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0.3011789924973205</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0.70953912111468376</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0.77063236870310814</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>0.59699892818863887</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>0.45766345123258301</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0.49624866023579856</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0.48767416934619512</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0.84244372990353711</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0.86923901393354785</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>0.48981779206859594</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>0.72668810289389063</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>0.91318327974276536</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>0.59592711682743837</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>0.45551982851018219</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>0.54876741693461939</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>0.87674169346195063</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>0.44480171489817794</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>0.947481243301179</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>0.99678456591639863</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>0.73847802786709527</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>0.54019292604501612</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>0.92604501607717027</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>0.78242229367631289</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>0.714898177920686</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>0.90782422293676324</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>0.41800643086816724</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>0.40943193997856381</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>0.6538049303322615</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>0.57663451232583074</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>0.42015005359056806</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1378,199 +1873,199 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="71"/>
                 <c:pt idx="0">
-                  <c:v>-9.7274970860700791E-2</c:v>
+                  <c:v>0.1877937841805371</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-5.986681386425944E-2</c:v>
+                  <c:v>0.46627169768356969</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.1831520849188856</c:v>
+                  <c:v>0.15401402503330097</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.31566346721885369</c:v>
+                  <c:v>-8.2966415647052996E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.22561490928544745</c:v>
+                  <c:v>-8.0053080273706292E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.12132444339874575</c:v>
+                  <c:v>-0.18219007055441891</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.9064368639894429E-2</c:v>
+                  <c:v>-0.32200196667481273</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.5096330313411993E-2</c:v>
+                  <c:v>-0.48762649722118473</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.11432672869973375</c:v>
+                  <c:v>-0.42859668088586472</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.16976245639454696</c:v>
+                  <c:v>-0.29253598880317838</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.23410257831601378</c:v>
+                  <c:v>-7.1805924426677922E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.11389029123075681</c:v>
+                  <c:v>0.12276658385680198</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.27422483387071978</c:v>
+                  <c:v>0.35634129191272074</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.16539843189828035</c:v>
+                  <c:v>0.40251016488394031</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-0.2660318514355115</c:v>
+                  <c:v>0.6499823008049922</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.23638714599352822</c:v>
+                  <c:v>0.37270311829563163</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-0.49074773227542845</c:v>
+                  <c:v>6.2363568731556615E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-0.22602306262176053</c:v>
+                  <c:v>-9.6331768367905926E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-4.9080204724352976E-2</c:v>
+                  <c:v>-0.40922509185493333</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-6.9935472701607396E-2</c:v>
+                  <c:v>-0.36470408508766483</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-3.678156442754487E-2</c:v>
+                  <c:v>-0.64557038467235983</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-6.9755941839338392E-2</c:v>
+                  <c:v>-0.39035746742197186</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.0100132677680174E-2</c:v>
+                  <c:v>-0.18672811494854619</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-0.13744232413694835</c:v>
+                  <c:v>-0.12127796780747488</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4.8671028644223159E-2</c:v>
+                  <c:v>4.2726795823512506E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.18208367667745565</c:v>
+                  <c:v>5.8670411735280086E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.40181593075828276</c:v>
+                  <c:v>7.1432691801798578E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.40036496811971922</c:v>
+                  <c:v>1.1014666069011244E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.5292711139433679</c:v>
+                  <c:v>0.11504147647164607</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.73383437435441012</c:v>
+                  <c:v>6.6472456379569236E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.38253744679175317</c:v>
+                  <c:v>0.10652405228776121</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.16586566928236712</c:v>
+                  <c:v>0.14937962817293723</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-4.1705034743514585E-2</c:v>
+                  <c:v>0.40649326652375867</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-6.597171116574185E-3</c:v>
+                  <c:v>0.23108013365793517</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-7.0109275609870084E-2</c:v>
+                  <c:v>0.12796207163768505</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-0.11401811737298594</c:v>
+                  <c:v>0.22817358826099599</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-9.7809135631584471E-2</c:v>
+                  <c:v>7.0912332040516182E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-0.17163357160046236</c:v>
+                  <c:v>-8.9379456812388666E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>-0.26478972741060985</c:v>
+                  <c:v>-0.36588865003538718</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-0.21365245340812178</c:v>
+                  <c:v>-0.16205311927206142</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>-0.33599639908752205</c:v>
+                  <c:v>-0.32073912181138986</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>-0.48043047059331601</c:v>
+                  <c:v>-0.31432674138231625</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>-0.2475126797411896</c:v>
+                  <c:v>-0.16046111942342989</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>6.5241974488085566E-2</c:v>
+                  <c:v>-5.7828124243944859E-2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.23998828202539371</c:v>
+                  <c:v>0.18660134279130239</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.10654591943023287</c:v>
+                  <c:v>0.18288590935742746</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.33912298543995689</c:v>
+                  <c:v>0.4615481532140136</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.38223841914049417</c:v>
+                  <c:v>0.35869732019948442</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.13910159240680017</c:v>
+                  <c:v>0.26196042006903419</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>-0.15707238100864601</c:v>
+                  <c:v>0.12467132923633227</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>-0.23574991803580619</c:v>
+                  <c:v>-4.1250886435076066E-2</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>-0.23942051704508158</c:v>
+                  <c:v>-0.14903892383910067</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>-0.46996433159873435</c:v>
+                  <c:v>-0.42752420639518218</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>-0.42561780273815464</c:v>
+                  <c:v>-0.43870683637437841</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>-0.36492713126341964</c:v>
+                  <c:v>-0.47791162805923354</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>-0.12862435499517394</c:v>
+                  <c:v>-0.24802126068435185</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>-1.1367315850588103E-2</c:v>
+                  <c:v>-0.19392000361721173</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.12264585087781692</c:v>
+                  <c:v>-2.2671070106898884E-2</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.37058779279430143</c:v>
+                  <c:v>0.19400286329330171</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.55419613236811061</c:v>
+                  <c:v>0.5218867347813364</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.75705834677855621</c:v>
+                  <c:v>0.71289966635871693</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.52788504252489699</c:v>
+                  <c:v>0.45158903053802463</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.34961949600983694</c:v>
+                  <c:v>0.49403166197486664</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.36907021205231311</c:v>
+                  <c:v>0.30377090123173667</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.38885146274019494</c:v>
+                  <c:v>0.51644899900445196</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1994,6 +2489,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2511,6 +3046,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3066,16 +4117,52 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>534737</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>93578</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>138546</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>17702</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>224590</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>66441</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>369455</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>115455</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A4D7E62-F589-4EFD-962F-8999834B902F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>588616</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>32003</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>278468</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>4866</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3096,7 +4183,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3402,10 +4489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29511164-784E-426F-9F87-CDB65DD6FF7F}">
-  <dimension ref="B1:L74"/>
+  <dimension ref="B1:Y74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3418,31 +4505,31 @@
     <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>4</v>
       </c>
       <c r="C1">
-        <v>300</v>
+        <v>350</v>
       </c>
       <c r="F1" t="s">
         <v>7</v>
       </c>
       <c r="G1">
         <f ca="1">MAX(F4:F74)</f>
-        <v>6.75</v>
-      </c>
-    </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
+        <v>6.9950000000000001</v>
+      </c>
+    </row>
+    <row r="2" spans="2:25" x14ac:dyDescent="0.3">
       <c r="F2" t="s">
         <v>8</v>
       </c>
       <c r="G2">
         <f ca="1">MIN(F4:F74)</f>
-        <v>2.085</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="3" spans="2:25" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>3</v>
       </c>
@@ -3466,13 +4553,13 @@
       </c>
       <c r="J3">
         <f ca="1">MAX(H4:H74)</f>
-        <v>0.75705834677855621</v>
+        <v>0.71289966635871693</v>
       </c>
       <c r="L3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:25" x14ac:dyDescent="0.3">
       <c r="C4">
         <v>0</v>
       </c>
@@ -3481,25 +4568,31 @@
       </c>
       <c r="E4">
         <f t="shared" ref="E4:E35" ca="1" si="0">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.66</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="F4">
         <f ca="1">(D4+E4)/2</f>
-        <v>5.33</v>
+        <v>3.7850000000000001</v>
       </c>
       <c r="G4">
-        <f ca="1">(F4-minval)/(maxval-minval)</f>
-        <v>0.69560557341907825</v>
+        <f t="shared" ref="G4:G35" ca="1" si="1">(F4-minval)/(maxval-minval)</f>
+        <v>6.8214804063860754E-2</v>
       </c>
       <c r="H4">
         <f ca="1">CORREL(G4:G21,$L$4:$L$21)</f>
-        <v>-9.7274970860700791E-2</v>
+        <v>0.1877937841805371</v>
       </c>
       <c r="L4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="W4" t="s">
+        <v>11</v>
+      </c>
+      <c r="X4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:25" x14ac:dyDescent="0.3">
       <c r="C5">
         <v>0.05</v>
       </c>
@@ -3508,25 +4601,31 @@
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6</v>
+        <v>4.8600000000000003</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F5:F68" ca="1" si="1">(D5+E5)/2</f>
-        <v>4.3</v>
+        <f t="shared" ref="F5:F68" ca="1" si="2">(D5+E5)/2</f>
+        <v>5.93</v>
       </c>
       <c r="G5">
-        <f ca="1">(F5-minval)/(maxval-minval)</f>
-        <v>0.47481243301178988</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.69085631349782284</v>
       </c>
       <c r="H5">
-        <f t="shared" ref="H5:H68" ca="1" si="2">CORREL(G5:G22,$L$4:$L$21)</f>
-        <v>-5.986681386425944E-2</v>
+        <f t="shared" ref="H5:H68" ca="1" si="3">CORREL(G5:G22,$L$4:$L$21)</f>
+        <v>0.46627169768356969</v>
       </c>
       <c r="L5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="W5">
+        <v>1</v>
+      </c>
+      <c r="X5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:25" x14ac:dyDescent="0.3">
       <c r="C6">
         <v>0.1</v>
       </c>
@@ -3535,25 +4634,31 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>3.32</v>
+        <v>4.42</v>
       </c>
       <c r="F6">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.71</v>
+      </c>
+      <c r="G6">
         <f t="shared" ca="1" si="1"/>
-        <v>5.16</v>
-      </c>
-      <c r="G6">
-        <f ca="1">(F6-minval)/(maxval-minval)</f>
-        <v>0.65916398713826374</v>
+        <v>0.62699564586357037</v>
       </c>
       <c r="H6">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.1831520849188856</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.15401402503330097</v>
       </c>
       <c r="L6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="W6">
+        <v>10</v>
+      </c>
+      <c r="X6">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="7" spans="2:25" x14ac:dyDescent="0.3">
       <c r="C7">
         <v>0.15</v>
       </c>
@@ -3562,25 +4667,31 @@
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>6.15</v>
+        <v>1.01</v>
       </c>
       <c r="F7">
+        <f t="shared" ca="1" si="2"/>
+        <v>4.0049999999999999</v>
+      </c>
+      <c r="G7">
         <f t="shared" ca="1" si="1"/>
-        <v>6.5750000000000002</v>
-      </c>
-      <c r="G7">
-        <f ca="1">(F7-minval)/(maxval-minval)</f>
-        <v>0.962486602357985</v>
+        <v>0.13207547169811321</v>
       </c>
       <c r="H7">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.31566346721885369</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-8.2966415647052996E-2</v>
       </c>
       <c r="L7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="W7">
+        <v>50</v>
+      </c>
+      <c r="X7">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="8" spans="2:25" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>0.2</v>
       </c>
@@ -3589,25 +4700,34 @@
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>1.19</v>
+        <v>3.13</v>
       </c>
       <c r="F8">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.0649999999999995</v>
+      </c>
+      <c r="G8">
         <f t="shared" ca="1" si="1"/>
-        <v>4.0949999999999998</v>
-      </c>
-      <c r="G8">
-        <f ca="1">(F8-minval)/(maxval-minval)</f>
-        <v>0.43086816720257232</v>
+        <v>0.43976777939042078</v>
       </c>
       <c r="H8">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.22561490928544745</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-8.0053080273706292E-2</v>
+      </c>
+      <c r="J8">
+        <v>60</v>
       </c>
       <c r="L8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="W8">
+        <v>100</v>
+      </c>
+      <c r="X8">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="9" spans="2:25" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>0.25</v>
       </c>
@@ -3616,25 +4736,34 @@
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5</v>
+        <v>4.8899999999999997</v>
       </c>
       <c r="F9">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.9450000000000003</v>
+      </c>
+      <c r="G9">
         <f t="shared" ca="1" si="1"/>
-        <v>4.25</v>
-      </c>
-      <c r="G9">
-        <f ca="1">(F9-minval)/(maxval-minval)</f>
-        <v>0.46409431939978563</v>
+        <v>0.69521044992743108</v>
       </c>
       <c r="H9">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.12132444339874575</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.18219007055441891</v>
+      </c>
+      <c r="J9">
+        <v>71</v>
       </c>
       <c r="L9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="W9">
+        <v>200</v>
+      </c>
+      <c r="X9">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="10" spans="2:25" x14ac:dyDescent="0.3">
       <c r="C10">
         <v>0.3</v>
       </c>
@@ -3643,25 +4772,34 @@
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>5.4</v>
+        <v>4.12</v>
       </c>
       <c r="F10">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.5600000000000005</v>
+      </c>
+      <c r="G10">
         <f t="shared" ca="1" si="1"/>
-        <v>6.2</v>
-      </c>
-      <c r="G10">
-        <f ca="1">(F10-minval)/(maxval-minval)</f>
-        <v>0.88210075026795287</v>
+        <v>0.58345428156748924</v>
       </c>
       <c r="H10">
-        <f t="shared" ca="1" si="2"/>
-        <v>9.9064368639894429E-2</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.32200196667481273</v>
+      </c>
+      <c r="J10">
+        <v>78</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="W10">
+        <v>250</v>
+      </c>
+      <c r="X10">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:25" x14ac:dyDescent="0.3">
       <c r="C11">
         <v>0.35</v>
       </c>
@@ -3670,25 +4808,34 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.92</v>
+        <v>1.9</v>
       </c>
       <c r="F11">
+        <f t="shared" ca="1" si="2"/>
+        <v>4.45</v>
+      </c>
+      <c r="G11">
         <f t="shared" ca="1" si="1"/>
-        <v>3.96</v>
-      </c>
-      <c r="G11">
-        <f ca="1">(F11-minval)/(maxval-minval)</f>
-        <v>0.40192926045016075</v>
+        <v>0.26124818577648773</v>
       </c>
       <c r="H11">
-        <f t="shared" ca="1" si="2"/>
-        <v>3.5096330313411993E-2</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.48762649722118473</v>
+      </c>
+      <c r="J11">
+        <v>86</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="W11">
+        <v>300</v>
+      </c>
+      <c r="X11">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="12" spans="2:25" x14ac:dyDescent="0.3">
       <c r="C12">
         <v>0.4</v>
       </c>
@@ -3697,25 +4844,37 @@
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.6</v>
+        <v>0.47</v>
       </c>
       <c r="F12">
+        <f t="shared" ca="1" si="2"/>
+        <v>3.7349999999999999</v>
+      </c>
+      <c r="G12">
         <f t="shared" ca="1" si="1"/>
-        <v>3.8</v>
-      </c>
-      <c r="G12">
-        <f ca="1">(F12-minval)/(maxval-minval)</f>
-        <v>0.36763129689174701</v>
+        <v>5.3701015965166916E-2</v>
       </c>
       <c r="H12">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.11432672869973375</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.42859668088586472</v>
+      </c>
+      <c r="J12">
+        <v>78</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="W12">
+        <v>350</v>
+      </c>
+      <c r="X12">
+        <v>0.7</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="2:25" x14ac:dyDescent="0.3">
       <c r="C13">
         <v>0.45</v>
       </c>
@@ -3724,25 +4883,28 @@
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>5.7</v>
+        <v>3.61</v>
       </c>
       <c r="F13">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.3049999999999997</v>
+      </c>
+      <c r="G13">
         <f t="shared" ca="1" si="1"/>
-        <v>6.35</v>
-      </c>
-      <c r="G13">
-        <f ca="1">(F13-minval)/(maxval-minval)</f>
-        <v>0.91425509110396563</v>
+        <v>0.50943396226415083</v>
       </c>
       <c r="H13">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.16976245639454696</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.29253598880317838</v>
+      </c>
+      <c r="J13">
+        <v>74</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:25" x14ac:dyDescent="0.3">
       <c r="C14">
         <v>0.5</v>
       </c>
@@ -3751,25 +4913,28 @@
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>6.29</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="F14">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.6950000000000003</v>
+      </c>
+      <c r="G14">
         <f t="shared" ca="1" si="1"/>
-        <v>6.6449999999999996</v>
-      </c>
-      <c r="G14">
-        <f ca="1">(F14-minval)/(maxval-minval)</f>
-        <v>0.97749196141479089</v>
+        <v>0.62264150943396235</v>
       </c>
       <c r="H14">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.23410257831601378</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-7.1805924426677922E-2</v>
+      </c>
+      <c r="J14">
+        <v>66</v>
       </c>
       <c r="L14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:25" x14ac:dyDescent="0.3">
       <c r="C15">
         <v>0.55000000000000004</v>
       </c>
@@ -3778,25 +4943,28 @@
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2200000000000002</v>
+        <v>4.21</v>
       </c>
       <c r="F15">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.6050000000000004</v>
+      </c>
+      <c r="G15">
         <f t="shared" ca="1" si="1"/>
-        <v>4.6100000000000003</v>
-      </c>
-      <c r="G15">
-        <f ca="1">(F15-minval)/(maxval-minval)</f>
-        <v>0.54126473740621661</v>
+        <v>0.59651669085631365</v>
       </c>
       <c r="H15">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.11389029123075681</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.12276658385680198</v>
+      </c>
+      <c r="J15">
+        <v>71</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:25" x14ac:dyDescent="0.3">
       <c r="C16">
         <v>0.6</v>
       </c>
@@ -3805,19 +4973,22 @@
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>5.54</v>
+        <v>1.85</v>
       </c>
       <c r="F16">
+        <f t="shared" ca="1" si="2"/>
+        <v>4.4249999999999998</v>
+      </c>
+      <c r="G16">
         <f t="shared" ca="1" si="1"/>
-        <v>6.27</v>
-      </c>
-      <c r="G16">
-        <f ca="1">(F16-minval)/(maxval-minval)</f>
-        <v>0.89710610932475876</v>
+        <v>0.25399129172714074</v>
       </c>
       <c r="H16">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.27422483387071978</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.35634129191272074</v>
+      </c>
+      <c r="J16">
+        <v>63</v>
       </c>
       <c r="L16">
         <v>1</v>
@@ -3832,19 +5003,22 @@
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="0"/>
-        <v>3.44</v>
+        <v>6.27</v>
       </c>
       <c r="F17">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.6349999999999998</v>
+      </c>
+      <c r="G17">
         <f t="shared" ca="1" si="1"/>
-        <v>5.22</v>
-      </c>
-      <c r="G17">
-        <f ca="1">(F17-minval)/(maxval-minval)</f>
-        <v>0.67202572347266876</v>
+        <v>0.89550072568940486</v>
       </c>
       <c r="H17">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.16539843189828035</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.40251016488394031</v>
+      </c>
+      <c r="J17">
+        <v>82</v>
       </c>
       <c r="L17">
         <v>1</v>
@@ -3859,19 +5033,22 @@
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="0"/>
-        <v>2.34</v>
+        <v>3.15</v>
       </c>
       <c r="F18">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.0750000000000002</v>
+      </c>
+      <c r="G18">
         <f t="shared" ca="1" si="1"/>
-        <v>4.67</v>
-      </c>
-      <c r="G18">
-        <f ca="1">(F18-minval)/(maxval-minval)</f>
-        <v>0.55412647374062163</v>
+        <v>0.44267053701015974</v>
       </c>
       <c r="H18">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.2660318514355115</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.6499823008049922</v>
+      </c>
+      <c r="J18">
+        <v>61</v>
       </c>
       <c r="L18">
         <v>1</v>
@@ -3886,19 +5063,22 @@
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="0"/>
-        <v>2.57</v>
+        <v>4.04</v>
       </c>
       <c r="F19">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.52</v>
+      </c>
+      <c r="G19">
         <f t="shared" ca="1" si="1"/>
-        <v>4.7850000000000001</v>
-      </c>
-      <c r="G19">
-        <f ca="1">(F19-minval)/(maxval-minval)</f>
-        <v>0.5787781350482315</v>
+        <v>0.57184325108853395</v>
       </c>
       <c r="H19">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.23638714599352822</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.37270311829563163</v>
+      </c>
+      <c r="J19">
+        <v>59</v>
       </c>
       <c r="L19">
         <v>1</v>
@@ -3913,19 +5093,23 @@
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="0"/>
-        <v>2.46</v>
+        <v>6.15</v>
       </c>
       <c r="F20">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.5750000000000002</v>
+      </c>
+      <c r="G20">
         <f t="shared" ca="1" si="1"/>
-        <v>4.7300000000000004</v>
-      </c>
-      <c r="G20">
-        <f ca="1">(F20-minval)/(maxval-minval)</f>
-        <v>0.56698821007502687</v>
+        <v>0.87808417997097243</v>
       </c>
       <c r="H20">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.49074773227542845</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>6.2363568731556615E-2</v>
+      </c>
+      <c r="J20">
+        <f>AVERAGE(J8:J19)</f>
+        <v>70.75</v>
       </c>
       <c r="L20">
         <v>1</v>
@@ -3940,19 +5124,19 @@
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="0"/>
-        <v>3.98</v>
+        <v>5.35</v>
       </c>
       <c r="F21">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.1749999999999998</v>
+      </c>
+      <c r="G21">
         <f t="shared" ca="1" si="1"/>
-        <v>5.49</v>
-      </c>
-      <c r="G21">
-        <f ca="1">(F21-minval)/(maxval-minval)</f>
-        <v>0.729903536977492</v>
+        <v>0.76197387518142223</v>
       </c>
       <c r="H21">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.22602306262176053</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-9.6331768367905926E-2</v>
       </c>
       <c r="L21">
         <v>1</v>
@@ -3967,19 +5151,19 @@
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="0"/>
-        <v>5.69</v>
+        <v>4.18</v>
       </c>
       <c r="F22">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.59</v>
+      </c>
+      <c r="G22">
         <f t="shared" ca="1" si="1"/>
-        <v>6.3450000000000006</v>
-      </c>
-      <c r="G22">
-        <f ca="1">(F22-minval)/(maxval-minval)</f>
-        <v>0.91318327974276536</v>
+        <v>0.59216255442670529</v>
       </c>
       <c r="H22">
-        <f t="shared" ca="1" si="2"/>
-        <v>-4.9080204724352976E-2</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.40922509185493333</v>
       </c>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.3">
@@ -3991,19 +5175,19 @@
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="0"/>
-        <v>3.42</v>
+        <v>5.58</v>
       </c>
       <c r="F23">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.29</v>
+      </c>
+      <c r="G23">
         <f t="shared" ca="1" si="1"/>
-        <v>5.21</v>
-      </c>
-      <c r="G23">
-        <f ca="1">(F23-minval)/(maxval-minval)</f>
-        <v>0.66988210075026799</v>
+        <v>0.79535558780841797</v>
       </c>
       <c r="H23">
-        <f t="shared" ca="1" si="2"/>
-        <v>-6.9935472701607396E-2</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.36470408508766483</v>
       </c>
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.3">
@@ -4015,19 +5199,19 @@
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="0"/>
-        <v>2.06</v>
+        <v>2.71</v>
       </c>
       <c r="F24">
+        <f t="shared" ca="1" si="2"/>
+        <v>4.8550000000000004</v>
+      </c>
+      <c r="G24">
         <f t="shared" ca="1" si="1"/>
-        <v>4.53</v>
-      </c>
-      <c r="G24">
-        <f ca="1">(F24-minval)/(maxval-minval)</f>
-        <v>0.52411575562700974</v>
+        <v>0.37880986937590727</v>
       </c>
       <c r="H24">
-        <f t="shared" ca="1" si="2"/>
-        <v>-3.678156442754487E-2</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.64557038467235983</v>
       </c>
     </row>
     <row r="25" spans="3:12" x14ac:dyDescent="0.3">
@@ -4039,19 +5223,19 @@
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="0"/>
-        <v>1.51</v>
+        <v>2.65</v>
       </c>
       <c r="F25">
+        <f t="shared" ca="1" si="2"/>
+        <v>4.8250000000000002</v>
+      </c>
+      <c r="G25">
         <f t="shared" ca="1" si="1"/>
-        <v>4.2549999999999999</v>
-      </c>
-      <c r="G25">
-        <f ca="1">(F25-minval)/(maxval-minval)</f>
-        <v>0.46516613076098606</v>
+        <v>0.37010159651669094</v>
       </c>
       <c r="H25">
-        <f t="shared" ca="1" si="2"/>
-        <v>-6.9755941839338392E-2</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.39035746742197186</v>
       </c>
     </row>
     <row r="26" spans="3:12" x14ac:dyDescent="0.3">
@@ -4063,19 +5247,19 @@
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="0"/>
-        <v>5.72</v>
+        <v>4.49</v>
       </c>
       <c r="F26">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.7450000000000001</v>
+      </c>
+      <c r="G26">
         <f t="shared" ca="1" si="1"/>
-        <v>6.3599999999999994</v>
-      </c>
-      <c r="G26">
-        <f ca="1">(F26-minval)/(maxval-minval)</f>
-        <v>0.9163987138263664</v>
+        <v>0.6371552975326561</v>
       </c>
       <c r="H26">
-        <f t="shared" ca="1" si="2"/>
-        <v>1.0100132677680174E-2</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.18672811494854619</v>
       </c>
     </row>
     <row r="27" spans="3:12" x14ac:dyDescent="0.3">
@@ -4087,19 +5271,19 @@
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="0"/>
-        <v>5.78</v>
+        <v>3</v>
       </c>
       <c r="F27">
+        <f t="shared" ca="1" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="G27">
         <f t="shared" ca="1" si="1"/>
-        <v>6.3900000000000006</v>
-      </c>
-      <c r="G27">
-        <f ca="1">(F27-minval)/(maxval-minval)</f>
-        <v>0.92282958199356924</v>
+        <v>0.42089985486211901</v>
       </c>
       <c r="H27">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.13744232413694835</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.12127796780747488</v>
       </c>
     </row>
     <row r="28" spans="3:12" x14ac:dyDescent="0.3">
@@ -4111,19 +5295,19 @@
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.81</v>
+        <v>4.6399999999999997</v>
       </c>
       <c r="F28">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.82</v>
+      </c>
+      <c r="G28">
         <f t="shared" ca="1" si="1"/>
-        <v>4.9050000000000002</v>
-      </c>
-      <c r="G28">
-        <f ca="1">(F28-minval)/(maxval-minval)</f>
-        <v>0.60450160771704187</v>
+        <v>0.65892597968069677</v>
       </c>
       <c r="H28">
-        <f t="shared" ca="1" si="2"/>
-        <v>4.8671028644223159E-2</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>4.2726795823512506E-2</v>
       </c>
     </row>
     <row r="29" spans="3:12" x14ac:dyDescent="0.3">
@@ -4135,19 +5319,19 @@
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="0"/>
-        <v>4.18</v>
+        <v>2.5</v>
       </c>
       <c r="F29">
+        <f t="shared" ca="1" si="2"/>
+        <v>4.75</v>
+      </c>
+      <c r="G29">
         <f t="shared" ca="1" si="1"/>
-        <v>5.59</v>
-      </c>
-      <c r="G29">
-        <f ca="1">(F29-minval)/(maxval-minval)</f>
-        <v>0.7513397642015005</v>
+        <v>0.34833091436865021</v>
       </c>
       <c r="H29">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.18208367667745565</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>5.8670411735280086E-2</v>
       </c>
     </row>
     <row r="30" spans="3:12" x14ac:dyDescent="0.3">
@@ -4159,19 +5343,19 @@
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="0"/>
-        <v>1.73</v>
+        <v>5.69</v>
       </c>
       <c r="F30">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.3450000000000006</v>
+      </c>
+      <c r="G30">
         <f t="shared" ca="1" si="1"/>
-        <v>4.3650000000000002</v>
-      </c>
-      <c r="G30">
-        <f ca="1">(F30-minval)/(maxval-minval)</f>
-        <v>0.48874598070739556</v>
+        <v>0.81132075471698128</v>
       </c>
       <c r="H30">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.40181593075828276</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>7.1432691801798578E-2</v>
       </c>
     </row>
     <row r="31" spans="3:12" x14ac:dyDescent="0.3">
@@ -4183,19 +5367,19 @@
       </c>
       <c r="E31">
         <f t="shared" ca="1" si="0"/>
-        <v>4.8600000000000003</v>
+        <v>6.48</v>
       </c>
       <c r="F31">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.74</v>
+      </c>
+      <c r="G31">
         <f t="shared" ca="1" si="1"/>
-        <v>5.93</v>
-      </c>
-      <c r="G31">
-        <f ca="1">(F31-minval)/(maxval-minval)</f>
-        <v>0.82422293676312963</v>
+        <v>0.92597968069666181</v>
       </c>
       <c r="H31">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.40036496811971922</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1.1014666069011244E-2</v>
       </c>
     </row>
     <row r="32" spans="3:12" x14ac:dyDescent="0.3">
@@ -4207,19 +5391,19 @@
       </c>
       <c r="E32">
         <f t="shared" ca="1" si="0"/>
-        <v>2.68</v>
+        <v>6.56</v>
       </c>
       <c r="F32">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.7799999999999994</v>
+      </c>
+      <c r="G32">
         <f t="shared" ca="1" si="1"/>
-        <v>4.84</v>
-      </c>
-      <c r="G32">
-        <f ca="1">(F32-minval)/(maxval-minval)</f>
-        <v>0.59056806002143625</v>
+        <v>0.93759071117561665</v>
       </c>
       <c r="H32">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.5292711139433679</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.11504147647164607</v>
       </c>
     </row>
     <row r="33" spans="3:8" x14ac:dyDescent="0.3">
@@ -4231,19 +5415,19 @@
       </c>
       <c r="E33">
         <f t="shared" ca="1" si="0"/>
-        <v>1.43</v>
+        <v>6.87</v>
       </c>
       <c r="F33">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.9350000000000005</v>
+      </c>
+      <c r="G33">
         <f t="shared" ca="1" si="1"/>
-        <v>4.2149999999999999</v>
-      </c>
-      <c r="G33">
-        <f ca="1">(F33-minval)/(maxval-minval)</f>
-        <v>0.45659163987138263</v>
+        <v>0.98258345428156757</v>
       </c>
       <c r="H33">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.73383437435441012</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>6.6472456379569236E-2</v>
       </c>
     </row>
     <row r="34" spans="3:8" x14ac:dyDescent="0.3">
@@ -4255,19 +5439,19 @@
       </c>
       <c r="E34">
         <f t="shared" ca="1" si="0"/>
-        <v>0.94</v>
+        <v>3.78</v>
       </c>
       <c r="F34">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.39</v>
+      </c>
+      <c r="G34">
         <f t="shared" ca="1" si="1"/>
-        <v>3.9699999999999998</v>
-      </c>
-      <c r="G34">
-        <f ca="1">(F34-minval)/(maxval-minval)</f>
-        <v>0.40407288317256157</v>
+        <v>0.5341074020319303</v>
       </c>
       <c r="H34">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.38253744679175317</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.10652405228776121</v>
       </c>
     </row>
     <row r="35" spans="3:8" x14ac:dyDescent="0.3">
@@ -4279,19 +5463,19 @@
       </c>
       <c r="E35">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6</v>
+        <v>6.83</v>
       </c>
       <c r="F35">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.915</v>
+      </c>
+      <c r="G35">
         <f t="shared" ca="1" si="1"/>
-        <v>4.3</v>
-      </c>
-      <c r="G35">
-        <f ca="1">(F35-minval)/(maxval-minval)</f>
-        <v>0.47481243301178988</v>
+        <v>0.97677793904208998</v>
       </c>
       <c r="H35">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.16586566928236712</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.14937962817293723</v>
       </c>
     </row>
     <row r="36" spans="3:8" x14ac:dyDescent="0.3">
@@ -4302,20 +5486,20 @@
         <v>7</v>
       </c>
       <c r="E36">
-        <f t="shared" ref="E36:E67" ca="1" si="3">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>2.54</v>
+        <f t="shared" ref="E36:E67" ca="1" si="4">RANDBETWEEN(350-noise,350+noise)/100</f>
+        <v>2.21</v>
       </c>
       <c r="F36">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.7699999999999996</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>4.6050000000000004</v>
       </c>
       <c r="G36">
-        <f ca="1">(F36-minval)/(maxval-minval)</f>
-        <v>0.57556270096463014</v>
+        <f t="shared" ref="G36:G67" ca="1" si="5">(F36-minval)/(maxval-minval)</f>
+        <v>0.30624092888243848</v>
       </c>
       <c r="H36">
-        <f t="shared" ca="1" si="2"/>
-        <v>-4.1705034743514585E-2</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.40649326652375867</v>
       </c>
     </row>
     <row r="37" spans="3:8" x14ac:dyDescent="0.3">
@@ -4326,20 +5510,20 @@
         <v>7</v>
       </c>
       <c r="E37">
+        <f t="shared" ca="1" si="4"/>
+        <v>3.25</v>
+      </c>
+      <c r="F37">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.125</v>
+      </c>
+      <c r="G37">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.45718432510885343</v>
+      </c>
+      <c r="H37">
         <f t="shared" ca="1" si="3"/>
-        <v>2.72</v>
-      </c>
-      <c r="F37">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.8600000000000003</v>
-      </c>
-      <c r="G37">
-        <f ca="1">(F37-minval)/(maxval-minval)</f>
-        <v>0.59485530546623799</v>
-      </c>
-      <c r="H37">
-        <f t="shared" ca="1" si="2"/>
-        <v>-6.597171116574185E-3</v>
+        <v>0.23108013365793517</v>
       </c>
     </row>
     <row r="38" spans="3:8" x14ac:dyDescent="0.3">
@@ -4350,20 +5534,20 @@
         <v>7</v>
       </c>
       <c r="E38">
+        <f t="shared" ca="1" si="4"/>
+        <v>5.97</v>
+      </c>
+      <c r="F38">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.4849999999999994</v>
+      </c>
+      <c r="G38">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.85195936139332351</v>
+      </c>
+      <c r="H38">
         <f t="shared" ca="1" si="3"/>
-        <v>3.68</v>
-      </c>
-      <c r="F38">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.34</v>
-      </c>
-      <c r="G38">
-        <f ca="1">(F38-minval)/(maxval-minval)</f>
-        <v>0.69774919614147912</v>
-      </c>
-      <c r="H38">
-        <f t="shared" ca="1" si="2"/>
-        <v>-7.0109275609870084E-2</v>
+        <v>0.12796207163768505</v>
       </c>
     </row>
     <row r="39" spans="3:8" x14ac:dyDescent="0.3">
@@ -4371,23 +5555,23 @@
         <v>1.75</v>
       </c>
       <c r="D39">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E39">
+        <f t="shared" ca="1" si="4"/>
+        <v>4.5</v>
+      </c>
+      <c r="F39">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.75</v>
+      </c>
+      <c r="G39">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.63860667634252544</v>
+      </c>
+      <c r="H39">
         <f t="shared" ca="1" si="3"/>
-        <v>1.17</v>
-      </c>
-      <c r="F39">
-        <f t="shared" ca="1" si="1"/>
-        <v>2.085</v>
-      </c>
-      <c r="G39">
-        <f ca="1">(F39-minval)/(maxval-minval)</f>
-        <v>0</v>
-      </c>
-      <c r="H39">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.11401811737298594</v>
+        <v>0.22817358826099599</v>
       </c>
     </row>
     <row r="40" spans="3:8" x14ac:dyDescent="0.3">
@@ -4395,23 +5579,23 @@
         <v>1.8</v>
       </c>
       <c r="D40">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E40">
+        <f t="shared" ca="1" si="4"/>
+        <v>3.04</v>
+      </c>
+      <c r="F40">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="G40">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.42670537010159643</v>
+      </c>
+      <c r="H40">
         <f t="shared" ca="1" si="3"/>
-        <v>2.89</v>
-      </c>
-      <c r="F40">
-        <f t="shared" ca="1" si="1"/>
-        <v>2.9450000000000003</v>
-      </c>
-      <c r="G40">
-        <f ca="1">(F40-minval)/(maxval-minval)</f>
-        <v>0.1843515541264738</v>
-      </c>
-      <c r="H40">
-        <f t="shared" ca="1" si="2"/>
-        <v>-9.7809135631584471E-2</v>
+        <v>7.0912332040516182E-2</v>
       </c>
     </row>
     <row r="41" spans="3:8" x14ac:dyDescent="0.3">
@@ -4419,23 +5603,23 @@
         <v>1.85</v>
       </c>
       <c r="D41">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E41">
+        <f t="shared" ca="1" si="4"/>
+        <v>6.41</v>
+      </c>
+      <c r="F41">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.7050000000000001</v>
+      </c>
+      <c r="G41">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.9158200290275762</v>
+      </c>
+      <c r="H41">
         <f t="shared" ca="1" si="3"/>
-        <v>1.17</v>
-      </c>
-      <c r="F41">
-        <f t="shared" ca="1" si="1"/>
-        <v>2.085</v>
-      </c>
-      <c r="G41">
-        <f ca="1">(F41-minval)/(maxval-minval)</f>
-        <v>0</v>
-      </c>
-      <c r="H41">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.17163357160046236</v>
+        <v>-8.9379456812388666E-2</v>
       </c>
     </row>
     <row r="42" spans="3:8" x14ac:dyDescent="0.3">
@@ -4443,23 +5627,23 @@
         <v>1.9</v>
       </c>
       <c r="D42">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E42">
+        <f t="shared" ca="1" si="4"/>
+        <v>3.25</v>
+      </c>
+      <c r="F42">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.125</v>
+      </c>
+      <c r="G42">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.45718432510885343</v>
+      </c>
+      <c r="H42">
         <f t="shared" ca="1" si="3"/>
-        <v>6.47</v>
-      </c>
-      <c r="F42">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.7349999999999994</v>
-      </c>
-      <c r="G42">
-        <f ca="1">(F42-minval)/(maxval-minval)</f>
-        <v>0.56806002143622714</v>
-      </c>
-      <c r="H42">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.26478972741060985</v>
+        <v>-0.36588865003538718</v>
       </c>
     </row>
     <row r="43" spans="3:8" x14ac:dyDescent="0.3">
@@ -4467,23 +5651,23 @@
         <v>1.95</v>
       </c>
       <c r="D43">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E43">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.2</v>
+      </c>
+      <c r="F43">
+        <f t="shared" ca="1" si="2"/>
+        <v>3.6</v>
+      </c>
+      <c r="G43">
+        <f t="shared" ca="1" si="5"/>
+        <v>1.4513788098693836E-2</v>
+      </c>
+      <c r="H43">
         <f t="shared" ca="1" si="3"/>
-        <v>3.99</v>
-      </c>
-      <c r="F43">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.4950000000000001</v>
-      </c>
-      <c r="G43">
-        <f ca="1">(F43-minval)/(maxval-minval)</f>
-        <v>0.30225080385852093</v>
-      </c>
-      <c r="H43">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.21365245340812178</v>
+        <v>-0.16205311927206142</v>
       </c>
     </row>
     <row r="44" spans="3:8" x14ac:dyDescent="0.3">
@@ -4491,23 +5675,23 @@
         <v>2</v>
       </c>
       <c r="D44">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E44">
+        <f t="shared" ca="1" si="4"/>
+        <v>5.74</v>
+      </c>
+      <c r="F44">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.37</v>
+      </c>
+      <c r="G44">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.81857764876632799</v>
+      </c>
+      <c r="H44">
         <f t="shared" ca="1" si="3"/>
-        <v>3.98</v>
-      </c>
-      <c r="F44">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.49</v>
-      </c>
-      <c r="G44">
-        <f ca="1">(F44-minval)/(maxval-minval)</f>
-        <v>0.3011789924973205</v>
-      </c>
-      <c r="H44">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.33599639908752205</v>
+        <v>-0.32073912181138986</v>
       </c>
     </row>
     <row r="45" spans="3:8" x14ac:dyDescent="0.3">
@@ -4518,20 +5702,20 @@
         <v>7</v>
       </c>
       <c r="E45">
+        <f t="shared" ca="1" si="4"/>
+        <v>3.72</v>
+      </c>
+      <c r="F45">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.36</v>
+      </c>
+      <c r="G45">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.52539912917271414</v>
+      </c>
+      <c r="H45">
         <f t="shared" ca="1" si="3"/>
-        <v>3.79</v>
-      </c>
-      <c r="F45">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.3949999999999996</v>
-      </c>
-      <c r="G45">
-        <f ca="1">(F45-minval)/(maxval-minval)</f>
-        <v>0.70953912111468376</v>
-      </c>
-      <c r="H45">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.48043047059331601</v>
+        <v>-0.31432674138231625</v>
       </c>
     </row>
     <row r="46" spans="3:8" x14ac:dyDescent="0.3">
@@ -4542,20 +5726,20 @@
         <v>7</v>
       </c>
       <c r="E46">
+        <f t="shared" ca="1" si="4"/>
+        <v>3.21</v>
+      </c>
+      <c r="F46">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.1050000000000004</v>
+      </c>
+      <c r="G46">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.45137880986937606</v>
+      </c>
+      <c r="H46">
         <f t="shared" ca="1" si="3"/>
-        <v>4.3600000000000003</v>
-      </c>
-      <c r="F46">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.68</v>
-      </c>
-      <c r="G46">
-        <f ca="1">(F46-minval)/(maxval-minval)</f>
-        <v>0.77063236870310814</v>
-      </c>
-      <c r="H46">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.2475126797411896</v>
+        <v>-0.16046111942342989</v>
       </c>
     </row>
     <row r="47" spans="3:8" x14ac:dyDescent="0.3">
@@ -4566,20 +5750,20 @@
         <v>7</v>
       </c>
       <c r="E47">
+        <f t="shared" ca="1" si="4"/>
+        <v>1.92</v>
+      </c>
+      <c r="F47">
+        <f t="shared" ca="1" si="2"/>
+        <v>4.46</v>
+      </c>
+      <c r="G47">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.26415094339622641</v>
+      </c>
+      <c r="H47">
         <f t="shared" ca="1" si="3"/>
-        <v>2.74</v>
-      </c>
-      <c r="F47">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.87</v>
-      </c>
-      <c r="G47">
-        <f ca="1">(F47-minval)/(maxval-minval)</f>
-        <v>0.59699892818863887</v>
-      </c>
-      <c r="H47">
-        <f t="shared" ca="1" si="2"/>
-        <v>6.5241974488085566E-2</v>
+        <v>-5.7828124243944859E-2</v>
       </c>
     </row>
     <row r="48" spans="3:8" x14ac:dyDescent="0.3">
@@ -4590,20 +5774,20 @@
         <v>7</v>
       </c>
       <c r="E48">
+        <f t="shared" ca="1" si="4"/>
+        <v>5.86</v>
+      </c>
+      <c r="F48">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.43</v>
+      </c>
+      <c r="G48">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.83599419448476042</v>
+      </c>
+      <c r="H48">
         <f t="shared" ca="1" si="3"/>
-        <v>1.44</v>
-      </c>
-      <c r="F48">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.22</v>
-      </c>
-      <c r="G48">
-        <f ca="1">(F48-minval)/(maxval-minval)</f>
-        <v>0.45766345123258301</v>
-      </c>
-      <c r="H48">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.23998828202539371</v>
+        <v>0.18660134279130239</v>
       </c>
     </row>
     <row r="49" spans="3:8" x14ac:dyDescent="0.3">
@@ -4614,20 +5798,20 @@
         <v>7</v>
       </c>
       <c r="E49">
+        <f t="shared" ca="1" si="4"/>
+        <v>2.39</v>
+      </c>
+      <c r="F49">
+        <f t="shared" ca="1" si="2"/>
+        <v>4.6950000000000003</v>
+      </c>
+      <c r="G49">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.33236574746008718</v>
+      </c>
+      <c r="H49">
         <f t="shared" ca="1" si="3"/>
-        <v>1.8</v>
-      </c>
-      <c r="F49">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="G49">
-        <f ca="1">(F49-minval)/(maxval-minval)</f>
-        <v>0.49624866023579856</v>
-      </c>
-      <c r="H49">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.10654591943023287</v>
+        <v>0.18288590935742746</v>
       </c>
     </row>
     <row r="50" spans="3:8" x14ac:dyDescent="0.3">
@@ -4638,20 +5822,20 @@
         <v>7</v>
       </c>
       <c r="E50">
+        <f t="shared" ca="1" si="4"/>
+        <v>3.37</v>
+      </c>
+      <c r="F50">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.1850000000000005</v>
+      </c>
+      <c r="G50">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.47460087082728608</v>
+      </c>
+      <c r="H50">
         <f t="shared" ca="1" si="3"/>
-        <v>1.72</v>
-      </c>
-      <c r="F50">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.3600000000000003</v>
-      </c>
-      <c r="G50">
-        <f ca="1">(F50-minval)/(maxval-minval)</f>
-        <v>0.48767416934619512</v>
-      </c>
-      <c r="H50">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.33912298543995689</v>
+        <v>0.4615481532140136</v>
       </c>
     </row>
     <row r="51" spans="3:8" x14ac:dyDescent="0.3">
@@ -4662,20 +5846,20 @@
         <v>7</v>
       </c>
       <c r="E51">
+        <f t="shared" ca="1" si="4"/>
+        <v>6.27</v>
+      </c>
+      <c r="F51">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.6349999999999998</v>
+      </c>
+      <c r="G51">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.89550072568940486</v>
+      </c>
+      <c r="H51">
         <f t="shared" ca="1" si="3"/>
-        <v>5.03</v>
-      </c>
-      <c r="F51">
-        <f t="shared" ca="1" si="1"/>
-        <v>6.0150000000000006</v>
-      </c>
-      <c r="G51">
-        <f ca="1">(F51-minval)/(maxval-minval)</f>
-        <v>0.84244372990353711</v>
-      </c>
-      <c r="H51">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.38223841914049417</v>
+        <v>0.35869732019948442</v>
       </c>
     </row>
     <row r="52" spans="3:8" x14ac:dyDescent="0.3">
@@ -4686,20 +5870,20 @@
         <v>7</v>
       </c>
       <c r="E52">
+        <f t="shared" ca="1" si="4"/>
+        <v>6.6</v>
+      </c>
+      <c r="F52">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.8</v>
+      </c>
+      <c r="G52">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.94339622641509424</v>
+      </c>
+      <c r="H52">
         <f t="shared" ca="1" si="3"/>
-        <v>6.5</v>
-      </c>
-      <c r="F52">
-        <f t="shared" ca="1" si="1"/>
-        <v>6.75</v>
-      </c>
-      <c r="G52">
-        <f ca="1">(F52-minval)/(maxval-minval)</f>
-        <v>1</v>
-      </c>
-      <c r="H52">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.13910159240680017</v>
+        <v>0.26196042006903419</v>
       </c>
     </row>
     <row r="53" spans="3:8" x14ac:dyDescent="0.3">
@@ -4710,20 +5894,20 @@
         <v>7</v>
       </c>
       <c r="E53">
+        <f t="shared" ca="1" si="4"/>
+        <v>4.51</v>
+      </c>
+      <c r="F53">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.7549999999999999</v>
+      </c>
+      <c r="G53">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.64005805515239478</v>
+      </c>
+      <c r="H53">
         <f t="shared" ca="1" si="3"/>
-        <v>5.28</v>
-      </c>
-      <c r="F53">
-        <f t="shared" ca="1" si="1"/>
-        <v>6.1400000000000006</v>
-      </c>
-      <c r="G53">
-        <f ca="1">(F53-minval)/(maxval-minval)</f>
-        <v>0.86923901393354785</v>
-      </c>
-      <c r="H53">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.15707238100864601</v>
+        <v>0.12467132923633227</v>
       </c>
     </row>
     <row r="54" spans="3:8" x14ac:dyDescent="0.3">
@@ -4734,20 +5918,20 @@
         <v>7</v>
       </c>
       <c r="E54">
+        <f t="shared" ca="1" si="4"/>
+        <v>2.16</v>
+      </c>
+      <c r="F54">
+        <f t="shared" ca="1" si="2"/>
+        <v>4.58</v>
+      </c>
+      <c r="G54">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.29898403483309149</v>
+      </c>
+      <c r="H54">
         <f t="shared" ca="1" si="3"/>
-        <v>1.74</v>
-      </c>
-      <c r="F54">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.37</v>
-      </c>
-      <c r="G54">
-        <f ca="1">(F54-minval)/(maxval-minval)</f>
-        <v>0.48981779206859594</v>
-      </c>
-      <c r="H54">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.23574991803580619</v>
+        <v>-4.1250886435076066E-2</v>
       </c>
     </row>
     <row r="55" spans="3:8" x14ac:dyDescent="0.3">
@@ -4758,20 +5942,20 @@
         <v>7</v>
       </c>
       <c r="E55">
+        <f t="shared" ca="1" si="4"/>
+        <v>5.2</v>
+      </c>
+      <c r="F55">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.1</v>
+      </c>
+      <c r="G55">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.74020319303338156</v>
+      </c>
+      <c r="H55">
         <f t="shared" ca="1" si="3"/>
-        <v>3.95</v>
-      </c>
-      <c r="F55">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.4749999999999996</v>
-      </c>
-      <c r="G55">
-        <f ca="1">(F55-minval)/(maxval-minval)</f>
-        <v>0.72668810289389063</v>
-      </c>
-      <c r="H55">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.23942051704508158</v>
+        <v>-0.14903892383910067</v>
       </c>
     </row>
     <row r="56" spans="3:8" x14ac:dyDescent="0.3">
@@ -4782,20 +5966,20 @@
         <v>7</v>
       </c>
       <c r="E56">
+        <f t="shared" ca="1" si="4"/>
+        <v>3.14</v>
+      </c>
+      <c r="F56">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.07</v>
+      </c>
+      <c r="G56">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.4412191582002904</v>
+      </c>
+      <c r="H56">
         <f t="shared" ca="1" si="3"/>
-        <v>5.69</v>
-      </c>
-      <c r="F56">
-        <f t="shared" ca="1" si="1"/>
-        <v>6.3450000000000006</v>
-      </c>
-      <c r="G56">
-        <f ca="1">(F56-minval)/(maxval-minval)</f>
-        <v>0.91318327974276536</v>
-      </c>
-      <c r="H56">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.46996433159873435</v>
+        <v>-0.42752420639518218</v>
       </c>
     </row>
     <row r="57" spans="3:8" x14ac:dyDescent="0.3">
@@ -4806,20 +5990,20 @@
         <v>7</v>
       </c>
       <c r="E57">
+        <f t="shared" ca="1" si="4"/>
+        <v>5.24</v>
+      </c>
+      <c r="F57">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.12</v>
+      </c>
+      <c r="G57">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.74600870827285926</v>
+      </c>
+      <c r="H57">
         <f t="shared" ca="1" si="3"/>
-        <v>2.73</v>
-      </c>
-      <c r="F57">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.8650000000000002</v>
-      </c>
-      <c r="G57">
-        <f ca="1">(F57-minval)/(maxval-minval)</f>
-        <v>0.59592711682743837</v>
-      </c>
-      <c r="H57">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.42561780273815464</v>
+        <v>-0.43870683637437841</v>
       </c>
     </row>
     <row r="58" spans="3:8" x14ac:dyDescent="0.3">
@@ -4830,20 +6014,20 @@
         <v>7</v>
       </c>
       <c r="E58">
+        <f t="shared" ca="1" si="4"/>
+        <v>5.96</v>
+      </c>
+      <c r="F58">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.48</v>
+      </c>
+      <c r="G58">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.85050798258345439</v>
+      </c>
+      <c r="H58">
         <f t="shared" ca="1" si="3"/>
-        <v>1.42</v>
-      </c>
-      <c r="F58">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.21</v>
-      </c>
-      <c r="G58">
-        <f ca="1">(F58-minval)/(maxval-minval)</f>
-        <v>0.45551982851018219</v>
-      </c>
-      <c r="H58">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.36492713126341964</v>
+        <v>-0.47791162805923354</v>
       </c>
     </row>
     <row r="59" spans="3:8" x14ac:dyDescent="0.3">
@@ -4854,20 +6038,20 @@
         <v>7</v>
       </c>
       <c r="E59">
+        <f t="shared" ca="1" si="4"/>
+        <v>1.29</v>
+      </c>
+      <c r="F59">
+        <f t="shared" ca="1" si="2"/>
+        <v>4.1449999999999996</v>
+      </c>
+      <c r="G59">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.17271407837445565</v>
+      </c>
+      <c r="H59">
         <f t="shared" ca="1" si="3"/>
-        <v>2.29</v>
-      </c>
-      <c r="F59">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.6449999999999996</v>
-      </c>
-      <c r="G59">
-        <f ca="1">(F59-minval)/(maxval-minval)</f>
-        <v>0.54876741693461939</v>
-      </c>
-      <c r="H59">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.12862435499517394</v>
+        <v>-0.24802126068435185</v>
       </c>
     </row>
     <row r="60" spans="3:8" x14ac:dyDescent="0.3">
@@ -4878,20 +6062,20 @@
         <v>7</v>
       </c>
       <c r="E60">
+        <f t="shared" ca="1" si="4"/>
+        <v>1.2</v>
+      </c>
+      <c r="F60">
+        <f t="shared" ca="1" si="2"/>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="G60">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.15965166908563128</v>
+      </c>
+      <c r="H60">
         <f t="shared" ca="1" si="3"/>
-        <v>5.35</v>
-      </c>
-      <c r="F60">
-        <f t="shared" ca="1" si="1"/>
-        <v>6.1749999999999998</v>
-      </c>
-      <c r="G60">
-        <f ca="1">(F60-minval)/(maxval-minval)</f>
-        <v>0.87674169346195063</v>
-      </c>
-      <c r="H60">
-        <f t="shared" ca="1" si="2"/>
-        <v>-1.1367315850588103E-2</v>
+        <v>-0.19392000361721173</v>
       </c>
     </row>
     <row r="61" spans="3:8" x14ac:dyDescent="0.3">
@@ -4902,20 +6086,20 @@
         <v>7</v>
       </c>
       <c r="E61">
+        <f t="shared" ca="1" si="4"/>
+        <v>2.15</v>
+      </c>
+      <c r="F61">
+        <f t="shared" ca="1" si="2"/>
+        <v>4.5750000000000002</v>
+      </c>
+      <c r="G61">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.29753265602322215</v>
+      </c>
+      <c r="H61">
         <f t="shared" ca="1" si="3"/>
-        <v>1.32</v>
-      </c>
-      <c r="F61">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.16</v>
-      </c>
-      <c r="G61">
-        <f ca="1">(F61-minval)/(maxval-minval)</f>
-        <v>0.44480171489817794</v>
-      </c>
-      <c r="H61">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.12264585087781692</v>
+        <v>-2.2671070106898884E-2</v>
       </c>
     </row>
     <row r="62" spans="3:8" x14ac:dyDescent="0.3">
@@ -4926,20 +6110,20 @@
         <v>7</v>
       </c>
       <c r="E62">
+        <f t="shared" ca="1" si="4"/>
+        <v>5.46</v>
+      </c>
+      <c r="F62">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.23</v>
+      </c>
+      <c r="G62">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.77793904208998554</v>
+      </c>
+      <c r="H62">
         <f t="shared" ca="1" si="3"/>
-        <v>6.01</v>
-      </c>
-      <c r="F62">
-        <f t="shared" ca="1" si="1"/>
-        <v>6.5049999999999999</v>
-      </c>
-      <c r="G62">
-        <f ca="1">(F62-minval)/(maxval-minval)</f>
-        <v>0.947481243301179</v>
-      </c>
-      <c r="H62">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.37058779279430143</v>
+        <v>0.19400286329330171</v>
       </c>
     </row>
     <row r="63" spans="3:8" x14ac:dyDescent="0.3">
@@ -4950,20 +6134,20 @@
         <v>7</v>
       </c>
       <c r="E63">
+        <f t="shared" ca="1" si="4"/>
+        <v>6.93</v>
+      </c>
+      <c r="F63">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.9649999999999999</v>
+      </c>
+      <c r="G63">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.99129172714078362</v>
+      </c>
+      <c r="H63">
         <f t="shared" ca="1" si="3"/>
-        <v>6.47</v>
-      </c>
-      <c r="F63">
-        <f t="shared" ca="1" si="1"/>
-        <v>6.7349999999999994</v>
-      </c>
-      <c r="G63">
-        <f ca="1">(F63-minval)/(maxval-minval)</f>
-        <v>0.99678456591639863</v>
-      </c>
-      <c r="H63">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.55419613236811061</v>
+        <v>0.5218867347813364</v>
       </c>
     </row>
     <row r="64" spans="3:8" x14ac:dyDescent="0.3">
@@ -4974,20 +6158,20 @@
         <v>7</v>
       </c>
       <c r="E64">
+        <f t="shared" ca="1" si="4"/>
+        <v>6.14</v>
+      </c>
+      <c r="F64">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.57</v>
+      </c>
+      <c r="G64">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.87663280116110309</v>
+      </c>
+      <c r="H64">
         <f t="shared" ca="1" si="3"/>
-        <v>4.0599999999999996</v>
-      </c>
-      <c r="F64">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.5299999999999994</v>
-      </c>
-      <c r="G64">
-        <f ca="1">(F64-minval)/(maxval-minval)</f>
-        <v>0.73847802786709527</v>
-      </c>
-      <c r="H64">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.75705834677855621</v>
+        <v>0.71289966635871693</v>
       </c>
     </row>
     <row r="65" spans="3:8" x14ac:dyDescent="0.3">
@@ -4998,20 +6182,20 @@
         <v>7</v>
       </c>
       <c r="E65">
+        <f t="shared" ca="1" si="4"/>
+        <v>3.89</v>
+      </c>
+      <c r="F65">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.4450000000000003</v>
+      </c>
+      <c r="G65">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.55007256894049361</v>
+      </c>
+      <c r="H65">
         <f t="shared" ca="1" si="3"/>
-        <v>2.21</v>
-      </c>
-      <c r="F65">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.6050000000000004</v>
-      </c>
-      <c r="G65">
-        <f ca="1">(F65-minval)/(maxval-minval)</f>
-        <v>0.54019292604501612</v>
-      </c>
-      <c r="H65">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.52788504252489699</v>
+        <v>0.45158903053802463</v>
       </c>
     </row>
     <row r="66" spans="3:8" x14ac:dyDescent="0.3">
@@ -5022,20 +6206,20 @@
         <v>7</v>
       </c>
       <c r="E66">
+        <f t="shared" ca="1" si="4"/>
+        <v>2.77</v>
+      </c>
+      <c r="F66">
+        <f t="shared" ca="1" si="2"/>
+        <v>4.8849999999999998</v>
+      </c>
+      <c r="G66">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.38751814223512332</v>
+      </c>
+      <c r="H66">
         <f t="shared" ca="1" si="3"/>
-        <v>5.81</v>
-      </c>
-      <c r="F66">
-        <f t="shared" ca="1" si="1"/>
-        <v>6.4049999999999994</v>
-      </c>
-      <c r="G66">
-        <f ca="1">(F66-minval)/(maxval-minval)</f>
-        <v>0.92604501607717027</v>
-      </c>
-      <c r="H66">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.34961949600983694</v>
+        <v>0.49403166197486664</v>
       </c>
     </row>
     <row r="67" spans="3:8" x14ac:dyDescent="0.3">
@@ -5046,20 +6230,20 @@
         <v>7</v>
       </c>
       <c r="E67">
+        <f t="shared" ca="1" si="4"/>
+        <v>6.89</v>
+      </c>
+      <c r="F67">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.9450000000000003</v>
+      </c>
+      <c r="G67">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.98548621190130625</v>
+      </c>
+      <c r="H67">
         <f t="shared" ca="1" si="3"/>
-        <v>4.47</v>
-      </c>
-      <c r="F67">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.7349999999999994</v>
-      </c>
-      <c r="G67">
-        <f ca="1">(F67-minval)/(maxval-minval)</f>
-        <v>0.78242229367631289</v>
-      </c>
-      <c r="H67">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.36907021205231311</v>
+        <v>0.30377090123173667</v>
       </c>
     </row>
     <row r="68" spans="3:8" x14ac:dyDescent="0.3">
@@ -5070,20 +6254,20 @@
         <v>7</v>
       </c>
       <c r="E68">
-        <f t="shared" ref="E68:E74" ca="1" si="4">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.84</v>
+        <f t="shared" ref="E68:E74" ca="1" si="6">RANDBETWEEN(350-noise,350+noise)/100</f>
+        <v>5.32</v>
       </c>
       <c r="F68">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.42</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>6.16</v>
       </c>
       <c r="G68">
-        <f ca="1">(F68-minval)/(maxval-minval)</f>
-        <v>0.714898177920686</v>
+        <f t="shared" ref="G68:G99" ca="1" si="7">(F68-minval)/(maxval-minval)</f>
+        <v>0.75761973875181421</v>
       </c>
       <c r="H68">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.38885146274019494</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.51644899900445196</v>
       </c>
     </row>
     <row r="69" spans="3:8" x14ac:dyDescent="0.3">
@@ -5094,16 +6278,16 @@
         <v>7</v>
       </c>
       <c r="E69">
-        <f t="shared" ca="1" si="4"/>
-        <v>5.64</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>6.99</v>
       </c>
       <c r="F69">
-        <f t="shared" ref="F69:F74" ca="1" si="5">(D69+E69)/2</f>
-        <v>6.32</v>
+        <f t="shared" ref="F69:F74" ca="1" si="8">(D69+E69)/2</f>
+        <v>6.9950000000000001</v>
       </c>
       <c r="G69">
-        <f ca="1">(F69-minval)/(maxval-minval)</f>
-        <v>0.90782422293676324</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="3:8" x14ac:dyDescent="0.3">
@@ -5114,16 +6298,16 @@
         <v>7</v>
       </c>
       <c r="E70">
-        <f t="shared" ca="1" si="4"/>
-        <v>1.07</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.76</v>
       </c>
       <c r="F70">
-        <f t="shared" ca="1" si="5"/>
-        <v>4.0350000000000001</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>3.88</v>
       </c>
       <c r="G70">
-        <f ca="1">(F70-minval)/(maxval-minval)</f>
-        <v>0.41800643086816724</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>9.5791001451378824E-2</v>
       </c>
     </row>
     <row r="71" spans="3:8" x14ac:dyDescent="0.3">
@@ -5134,16 +6318,16 @@
         <v>7</v>
       </c>
       <c r="E71">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.99</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>3.67</v>
       </c>
       <c r="F71">
-        <f t="shared" ca="1" si="5"/>
-        <v>3.9950000000000001</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>5.335</v>
       </c>
       <c r="G71">
-        <f ca="1">(F71-minval)/(maxval-minval)</f>
-        <v>0.40943193997856381</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.51814223512336721</v>
       </c>
     </row>
     <row r="72" spans="3:8" x14ac:dyDescent="0.3">
@@ -5154,16 +6338,16 @@
         <v>7</v>
       </c>
       <c r="E72">
-        <f t="shared" ca="1" si="4"/>
-        <v>3.27</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.93</v>
       </c>
       <c r="F72">
-        <f t="shared" ca="1" si="5"/>
-        <v>5.1349999999999998</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>3.9649999999999999</v>
       </c>
       <c r="G72">
-        <f ca="1">(F72-minval)/(maxval-minval)</f>
-        <v>0.6538049303322615</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.1204644412191582</v>
       </c>
     </row>
     <row r="73" spans="3:8" x14ac:dyDescent="0.3">
@@ -5174,16 +6358,16 @@
         <v>7</v>
       </c>
       <c r="E73">
-        <f t="shared" ca="1" si="4"/>
-        <v>2.5499999999999998</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>4.46</v>
       </c>
       <c r="F73">
-        <f t="shared" ca="1" si="5"/>
-        <v>4.7750000000000004</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>5.73</v>
       </c>
       <c r="G73">
-        <f ca="1">(F73-minval)/(maxval-minval)</f>
-        <v>0.57663451232583074</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.63280116110304807</v>
       </c>
     </row>
     <row r="74" spans="3:8" x14ac:dyDescent="0.3">
@@ -5194,16 +6378,16 @@
         <v>7</v>
       </c>
       <c r="E74">
-        <f t="shared" ca="1" si="4"/>
-        <v>1.0900000000000001</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.1</v>
       </c>
       <c r="F74">
-        <f t="shared" ca="1" si="5"/>
-        <v>4.0449999999999999</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>3.55</v>
       </c>
       <c r="G74">
-        <f ca="1">(F74-minval)/(maxval-minval)</f>
-        <v>0.42015005359056806</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
*** Restructuring the Docs Directory ***
</commit_message>
<xml_diff>
--- a/docs/LIDAR/Rain Simulation (cross correlation).xlsx
+++ b/docs/LIDAR/Rain Simulation (cross correlation).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnp\Dropbox\Programming\c++\LIDAR\docs\LIDAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85267E87-777B-47CD-89CC-D14F68928733}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{956C67C8-D132-434D-B58D-9E1A87A1505A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{6F829C6E-AC9C-4B9E-9DA9-8841D05EEE17}"/>
   </bookViews>
@@ -21,6 +21,7 @@
     <definedName name="noise">Sheet1!$C$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1423,217 +1424,217 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="71"/>
                 <c:pt idx="0">
-                  <c:v>6.8214804063860754E-2</c:v>
+                  <c:v>0.84917355371900816</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.69085631349782284</c:v>
+                  <c:v>0.95867768595041336</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.62699564586357037</c:v>
+                  <c:v>0.99793388429752072</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.13207547169811321</c:v>
+                  <c:v>0.90909090909090917</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.43976777939042078</c:v>
+                  <c:v>0.82851239669421484</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.69521044992743108</c:v>
+                  <c:v>0.98140495867768596</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.58345428156748924</c:v>
+                  <c:v>0.81198347107438018</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.26124818577648773</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.3701015965166916E-2</c:v>
+                  <c:v>0.97520661157024768</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.50943396226415083</c:v>
+                  <c:v>0.96694214876033058</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.62264150943396235</c:v>
+                  <c:v>0.89256198347107452</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.59651669085631365</c:v>
+                  <c:v>0.82851239669421484</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.25399129172714074</c:v>
+                  <c:v>0.90082644628099162</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.89550072568940486</c:v>
+                  <c:v>0.8450413223140496</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.44267053701015974</c:v>
+                  <c:v>0.81818181818181834</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.57184325108853395</c:v>
+                  <c:v>0.84710743801652888</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.87808417997097243</c:v>
+                  <c:v>0.94008264462809932</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.76197387518142223</c:v>
+                  <c:v>0.84090909090909094</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.59216255442670529</c:v>
+                  <c:v>0.92768595041322321</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.79535558780841797</c:v>
+                  <c:v>0.88636363636363624</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.37880986937590727</c:v>
+                  <c:v>0.91735537190082639</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.37010159651669094</c:v>
+                  <c:v>0.9772727272727274</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.6371552975326561</c:v>
+                  <c:v>0.80785123966942152</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.42089985486211901</c:v>
+                  <c:v>0.99586776859504145</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.65892597968069677</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.34833091436865021</c:v>
+                  <c:v>0.90495867768595029</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.81132075471698128</c:v>
+                  <c:v>0.97933884297520668</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.92597968069666181</c:v>
+                  <c:v>0.99380165289256217</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.93759071117561665</c:v>
+                  <c:v>0.94008264462809932</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.98258345428156757</c:v>
+                  <c:v>0.94214876033057859</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.5341074020319303</c:v>
+                  <c:v>0.10537190082644624</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.97677793904208998</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.30624092888243848</c:v>
+                  <c:v>0.16528925619834708</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.45718432510885343</c:v>
+                  <c:v>2.8925619834710679E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.85195936139332351</c:v>
+                  <c:v>9.0909090909090814E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.63860667634252544</c:v>
+                  <c:v>5.371900826446277E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.42670537010159643</c:v>
+                  <c:v>0.85537190082644643</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.9158200290275762</c:v>
+                  <c:v>0.99173553719008278</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.45718432510885343</c:v>
+                  <c:v>0.89876033057851235</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1.4513788098693836E-2</c:v>
+                  <c:v>0.97107438016528913</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.81857764876632799</c:v>
+                  <c:v>0.91528925619834711</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.52539912917271414</c:v>
+                  <c:v>0.80785123966942152</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.45137880986937606</c:v>
+                  <c:v>0.91735537190082639</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.26415094339622641</c:v>
+                  <c:v>0.88636363636363624</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.83599419448476042</c:v>
+                  <c:v>0.96900826446280985</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.33236574746008718</c:v>
+                  <c:v>0.99380165289256217</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.47460087082728608</c:v>
+                  <c:v>0.84710743801652888</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.89550072568940486</c:v>
+                  <c:v>0.90909090909090917</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.94339622641509424</c:v>
+                  <c:v>0.97107438016528913</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.64005805515239478</c:v>
+                  <c:v>0.91322314049586784</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.29898403483309149</c:v>
+                  <c:v>0.79752066115702469</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.74020319303338156</c:v>
+                  <c:v>0.87396694214876047</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.4412191582002904</c:v>
+                  <c:v>0.97107438016528913</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.74600870827285926</c:v>
+                  <c:v>0.86363636363636365</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.85050798258345439</c:v>
+                  <c:v>0.92561983471074394</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.17271407837445565</c:v>
+                  <c:v>0.86157024793388426</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.15965166908563128</c:v>
+                  <c:v>0.84297520661157033</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.29753265602322215</c:v>
+                  <c:v>0.93595041322314043</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.77793904208998554</c:v>
+                  <c:v>0.96280991735537191</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.99129172714078362</c:v>
+                  <c:v>0.84297520661157033</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.87663280116110309</c:v>
+                  <c:v>0.85743801652892571</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.55007256894049361</c:v>
+                  <c:v>0.97314049586776885</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.38751814223512332</c:v>
+                  <c:v>0.96280991735537191</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.98548621190130625</c:v>
+                  <c:v>0.83471074380165278</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.75761973875181421</c:v>
+                  <c:v>0.87396694214876047</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>1</c:v>
+                  <c:v>0.85743801652892571</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>9.5791001451378824E-2</c:v>
+                  <c:v>0.87603305785123975</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.51814223512336721</c:v>
+                  <c:v>0.84917355371900816</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.1204644412191582</c:v>
+                  <c:v>0.89462809917355379</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.63280116110304807</c:v>
+                  <c:v>0.9070247933884299</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0</c:v>
+                  <c:v>0.91115702479338845</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1873,199 +1874,199 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="71"/>
                 <c:pt idx="0">
-                  <c:v>0.1877937841805371</c:v>
+                  <c:v>-0.13924177746935876</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.46627169768356969</c:v>
+                  <c:v>-0.25480856734589319</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.15401402503330097</c:v>
+                  <c:v>-1.7840084605017296E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-8.2966415647052996E-2</c:v>
+                  <c:v>0.23940682145254222</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-8.0053080273706292E-2</c:v>
+                  <c:v>0.49856707812953294</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.18219007055441891</c:v>
+                  <c:v>0.38634133582289881</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.32200196667481273</c:v>
+                  <c:v>0.36583264521612591</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.48762649722118473</c:v>
+                  <c:v>0.42896369582903882</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.42859668088586472</c:v>
+                  <c:v>0.31532722631346422</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.29253598880317838</c:v>
+                  <c:v>0.12662571778220347</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-7.1805924426677922E-2</c:v>
+                  <c:v>-0.10252080492390975</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.12276658385680198</c:v>
+                  <c:v>0.17196126764505287</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.35634129191272074</c:v>
+                  <c:v>-4.652010078885048E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.40251016488394031</c:v>
+                  <c:v>-0.2181441280162712</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.6499823008049922</c:v>
+                  <c:v>-0.27925209943895146</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.37270311829563163</c:v>
+                  <c:v>-0.34951124335203593</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.2363568731556615E-2</c:v>
+                  <c:v>-0.40156007611418992</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-9.6331768367905926E-2</c:v>
+                  <c:v>-0.50154438906052379</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-0.40922509185493333</c:v>
+                  <c:v>-0.5311957193750142</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-0.36470408508766483</c:v>
+                  <c:v>-0.28350768390067493</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-0.64557038467235983</c:v>
+                  <c:v>-1.2570813895303259E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-0.39035746742197186</c:v>
+                  <c:v>0.2181665254695902</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-0.18672811494854619</c:v>
+                  <c:v>0.49350835455313907</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-0.12127796780747488</c:v>
+                  <c:v>0.7410919198822381</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4.2726795823512506E-2</c:v>
+                  <c:v>0.99051379849270349</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>5.8670411735280086E-2</c:v>
+                  <c:v>0.77314666355519157</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7.1432691801798578E-2</c:v>
+                  <c:v>0.4838390338424548</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.1014666069011244E-2</c:v>
+                  <c:v>0.26960441114580841</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.11504147647164607</c:v>
+                  <c:v>-5.0186971546129821E-3</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>6.6472456379569236E-2</c:v>
+                  <c:v>-0.25642581948010973</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.10652405228776121</c:v>
+                  <c:v>-0.4828862704247891</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.14937962817293723</c:v>
+                  <c:v>-0.43191253808407526</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.40649326652375867</c:v>
+                  <c:v>-0.33672075738205337</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.23108013365793517</c:v>
+                  <c:v>-0.31466327287112095</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.12796207163768505</c:v>
+                  <c:v>-0.26425442241738445</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.22817358826099599</c:v>
+                  <c:v>-0.13832789870435269</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>7.0912332040516182E-2</c:v>
+                  <c:v>-0.1431499632721327</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-8.9379456812388666E-2</c:v>
+                  <c:v>-0.20843954033548764</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>-0.36588865003538718</c:v>
+                  <c:v>-0.36663040301010086</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-0.16205311927206142</c:v>
+                  <c:v>-3.976526620841471E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>-0.32073912181138986</c:v>
+                  <c:v>0.18922361658111589</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>-0.31432674138231625</c:v>
+                  <c:v>-3.9801889730957433E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>-0.16046111942342989</c:v>
+                  <c:v>8.2127981537410591E-2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>-5.7828124243944859E-2</c:v>
+                  <c:v>0.13501497426859002</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.18660134279130239</c:v>
+                  <c:v>0.29489844238856366</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.18288590935742746</c:v>
+                  <c:v>0.19878183280675699</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.4615481532140136</c:v>
+                  <c:v>-3.9736745314926096E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.35869732019948442</c:v>
+                  <c:v>-2.998773752251637E-3</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.26196042006903419</c:v>
+                  <c:v>4.438442905181886E-3</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.12467132923633227</c:v>
+                  <c:v>8.7680642090914182E-2</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>-4.1250886435076066E-2</c:v>
+                  <c:v>-0.21243195293665049</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>-0.14903892383910067</c:v>
+                  <c:v>-0.44962377747724597</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>-0.42752420639518218</c:v>
+                  <c:v>-0.17238356497697213</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>-0.43870683637437841</c:v>
+                  <c:v>-1.8441523356356973E-3</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>-0.47791162805923354</c:v>
+                  <c:v>-1.5367497398268893E-2</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>-0.24802126068435185</c:v>
+                  <c:v>-0.10439088410218882</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>-0.19392000361721173</c:v>
+                  <c:v>0.29081624250727883</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>-2.2671070106898884E-2</c:v>
+                  <c:v>0.59175091331526297</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.19400286329330171</c:v>
+                  <c:v>0.32463061034782065</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.5218867347813364</c:v>
+                  <c:v>9.5749083177827751E-2</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.71289966635871693</c:v>
+                  <c:v>6.5516611112358916E-2</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.45158903053802463</c:v>
+                  <c:v>6.5710329107352861E-2</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.49403166197486664</c:v>
+                  <c:v>-0.36760226344226715</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.30377090123173667</c:v>
+                  <c:v>-0.75191000825309684</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.51644899900445196</c:v>
+                  <c:v>-0.55109859209697132</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4117,16 +4118,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>138546</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>17702</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>438728</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>2307</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>369455</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>115455</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>61576</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>100061</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4153,16 +4154,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>588616</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>32003</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>503950</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>24306</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>278468</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>4866</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>193803</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>181897</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4492,7 +4493,7 @@
   <dimension ref="B1:Y74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4510,14 +4511,14 @@
         <v>4</v>
       </c>
       <c r="C1">
-        <v>350</v>
+        <v>50</v>
       </c>
       <c r="F1" t="s">
         <v>7</v>
       </c>
       <c r="G1">
         <f ca="1">MAX(F4:F74)</f>
-        <v>6.9950000000000001</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="2" spans="2:25" x14ac:dyDescent="0.3">
@@ -4526,7 +4527,7 @@
       </c>
       <c r="G2">
         <f ca="1">MIN(F4:F74)</f>
-        <v>3.55</v>
+        <v>3.08</v>
       </c>
     </row>
     <row r="3" spans="2:25" x14ac:dyDescent="0.3">
@@ -4553,7 +4554,7 @@
       </c>
       <c r="J3">
         <f ca="1">MAX(H4:H74)</f>
-        <v>0.71289966635871693</v>
+        <v>0.99051379849270349</v>
       </c>
       <c r="L3" t="s">
         <v>5</v>
@@ -4568,19 +4569,19 @@
       </c>
       <c r="E4">
         <f t="shared" ref="E4:E35" ca="1" si="0">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>0.56999999999999995</v>
+        <v>3.27</v>
       </c>
       <c r="F4">
         <f ca="1">(D4+E4)/2</f>
-        <v>3.7850000000000001</v>
+        <v>5.1349999999999998</v>
       </c>
       <c r="G4">
         <f t="shared" ref="G4:G35" ca="1" si="1">(F4-minval)/(maxval-minval)</f>
-        <v>6.8214804063860754E-2</v>
+        <v>0.84917355371900816</v>
       </c>
       <c r="H4">
         <f ca="1">CORREL(G4:G21,$L$4:$L$21)</f>
-        <v>0.1877937841805371</v>
+        <v>-0.13924177746935876</v>
       </c>
       <c r="L4">
         <v>1</v>
@@ -4601,19 +4602,19 @@
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>4.8600000000000003</v>
+        <v>3.8</v>
       </c>
       <c r="F5">
         <f t="shared" ref="F5:F68" ca="1" si="2">(D5+E5)/2</f>
-        <v>5.93</v>
+        <v>5.4</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.69085631349782284</v>
+        <v>0.95867768595041336</v>
       </c>
       <c r="H5">
         <f t="shared" ref="H5:H68" ca="1" si="3">CORREL(G5:G22,$L$4:$L$21)</f>
-        <v>0.46627169768356969</v>
+        <v>-0.25480856734589319</v>
       </c>
       <c r="L5">
         <v>1</v>
@@ -4634,19 +4635,19 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>4.42</v>
+        <v>3.99</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="2"/>
-        <v>5.71</v>
+        <v>5.4950000000000001</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.62699564586357037</v>
+        <v>0.99793388429752072</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="3"/>
-        <v>0.15401402503330097</v>
+        <v>-1.7840084605017296E-2</v>
       </c>
       <c r="L6">
         <v>1</v>
@@ -4667,19 +4668,19 @@
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>1.01</v>
+        <v>3.56</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="2"/>
-        <v>4.0049999999999999</v>
+        <v>5.28</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.13207547169811321</v>
+        <v>0.90909090909090917</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="3"/>
-        <v>-8.2966415647052996E-2</v>
+        <v>0.23940682145254222</v>
       </c>
       <c r="L7">
         <v>1</v>
@@ -4700,19 +4701,19 @@
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>3.13</v>
+        <v>3.17</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="2"/>
-        <v>5.0649999999999995</v>
+        <v>5.085</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.43976777939042078</v>
+        <v>0.82851239669421484</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="3"/>
-        <v>-8.0053080273706292E-2</v>
+        <v>0.49856707812953294</v>
       </c>
       <c r="J8">
         <v>60</v>
@@ -4736,19 +4737,19 @@
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>4.8899999999999997</v>
+        <v>3.91</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="2"/>
-        <v>5.9450000000000003</v>
+        <v>5.4550000000000001</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.69521044992743108</v>
+        <v>0.98140495867768596</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.18219007055441891</v>
+        <v>0.38634133582289881</v>
       </c>
       <c r="J9">
         <v>71</v>
@@ -4772,19 +4773,19 @@
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>4.12</v>
+        <v>3.09</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="2"/>
-        <v>5.5600000000000005</v>
+        <v>5.0449999999999999</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.58345428156748924</v>
+        <v>0.81198347107438018</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.32200196667481273</v>
+        <v>0.36583264521612591</v>
       </c>
       <c r="J10">
         <v>78</v>
@@ -4808,19 +4809,19 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>1.9</v>
+        <v>4</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="2"/>
-        <v>4.45</v>
+        <v>5.5</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="1"/>
-        <v>0.26124818577648773</v>
+        <v>1</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.48762649722118473</v>
+        <v>0.42896369582903882</v>
       </c>
       <c r="J11">
         <v>86</v>
@@ -4844,19 +4845,19 @@
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.47</v>
+        <v>3.88</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="2"/>
-        <v>3.7349999999999999</v>
+        <v>5.4399999999999995</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="1"/>
-        <v>5.3701015965166916E-2</v>
+        <v>0.97520661157024768</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.42859668088586472</v>
+        <v>0.31532722631346422</v>
       </c>
       <c r="J12">
         <v>78</v>
@@ -4883,19 +4884,19 @@
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>3.61</v>
+        <v>3.84</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="2"/>
-        <v>5.3049999999999997</v>
+        <v>5.42</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="1"/>
-        <v>0.50943396226415083</v>
+        <v>0.96694214876033058</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.29253598880317838</v>
+        <v>0.12662571778220347</v>
       </c>
       <c r="J13">
         <v>74</v>
@@ -4913,19 +4914,19 @@
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>4.3899999999999997</v>
+        <v>3.48</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="2"/>
-        <v>5.6950000000000003</v>
+        <v>5.24</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="1"/>
-        <v>0.62264150943396235</v>
+        <v>0.89256198347107452</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="3"/>
-        <v>-7.1805924426677922E-2</v>
+        <v>-0.10252080492390975</v>
       </c>
       <c r="J14">
         <v>66</v>
@@ -4943,19 +4944,19 @@
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>4.21</v>
+        <v>3.17</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="2"/>
-        <v>5.6050000000000004</v>
+        <v>5.085</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.59651669085631365</v>
+        <v>0.82851239669421484</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="3"/>
-        <v>0.12276658385680198</v>
+        <v>0.17196126764505287</v>
       </c>
       <c r="J15">
         <v>71</v>
@@ -4973,19 +4974,19 @@
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>1.85</v>
+        <v>3.52</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="2"/>
-        <v>4.4249999999999998</v>
+        <v>5.26</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="1"/>
-        <v>0.25399129172714074</v>
+        <v>0.90082644628099162</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.35634129191272074</v>
+        <v>-4.652010078885048E-2</v>
       </c>
       <c r="J16">
         <v>63</v>
@@ -5003,19 +5004,19 @@
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="0"/>
-        <v>6.27</v>
+        <v>3.25</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="2"/>
-        <v>6.6349999999999998</v>
+        <v>5.125</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.89550072568940486</v>
+        <v>0.8450413223140496</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="3"/>
-        <v>0.40251016488394031</v>
+        <v>-0.2181441280162712</v>
       </c>
       <c r="J17">
         <v>82</v>
@@ -5033,19 +5034,19 @@
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="0"/>
-        <v>3.15</v>
+        <v>3.12</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="2"/>
-        <v>5.0750000000000002</v>
+        <v>5.0600000000000005</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.44267053701015974</v>
+        <v>0.81818181818181834</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="3"/>
-        <v>0.6499823008049922</v>
+        <v>-0.27925209943895146</v>
       </c>
       <c r="J18">
         <v>61</v>
@@ -5063,19 +5064,19 @@
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="0"/>
-        <v>4.04</v>
+        <v>3.26</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="2"/>
-        <v>5.52</v>
+        <v>5.13</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.57184325108853395</v>
+        <v>0.84710743801652888</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="3"/>
-        <v>0.37270311829563163</v>
+        <v>-0.34951124335203593</v>
       </c>
       <c r="J19">
         <v>59</v>
@@ -5093,19 +5094,19 @@
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="0"/>
-        <v>6.15</v>
+        <v>3.71</v>
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="2"/>
-        <v>6.5750000000000002</v>
+        <v>5.3550000000000004</v>
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="1"/>
-        <v>0.87808417997097243</v>
+        <v>0.94008264462809932</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="3"/>
-        <v>6.2363568731556615E-2</v>
+        <v>-0.40156007611418992</v>
       </c>
       <c r="J20">
         <f>AVERAGE(J8:J19)</f>
@@ -5124,19 +5125,19 @@
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="0"/>
-        <v>5.35</v>
+        <v>3.23</v>
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="2"/>
-        <v>6.1749999999999998</v>
+        <v>5.1150000000000002</v>
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="1"/>
-        <v>0.76197387518142223</v>
+        <v>0.84090909090909094</v>
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="3"/>
-        <v>-9.6331768367905926E-2</v>
+        <v>-0.50154438906052379</v>
       </c>
       <c r="L21">
         <v>1</v>
@@ -5151,19 +5152,19 @@
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="0"/>
-        <v>4.18</v>
+        <v>3.65</v>
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="2"/>
-        <v>5.59</v>
+        <v>5.3250000000000002</v>
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.59216255442670529</v>
+        <v>0.92768595041322321</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.40922509185493333</v>
+        <v>-0.5311957193750142</v>
       </c>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.3">
@@ -5175,19 +5176,19 @@
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="0"/>
-        <v>5.58</v>
+        <v>3.45</v>
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="2"/>
-        <v>6.29</v>
+        <v>5.2249999999999996</v>
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.79535558780841797</v>
+        <v>0.88636363636363624</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.36470408508766483</v>
+        <v>-0.28350768390067493</v>
       </c>
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.3">
@@ -5199,19 +5200,19 @@
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="0"/>
-        <v>2.71</v>
+        <v>3.6</v>
       </c>
       <c r="F24">
         <f t="shared" ca="1" si="2"/>
-        <v>4.8550000000000004</v>
+        <v>5.3</v>
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.37880986937590727</v>
+        <v>0.91735537190082639</v>
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.64557038467235983</v>
+        <v>-1.2570813895303259E-2</v>
       </c>
     </row>
     <row r="25" spans="3:12" x14ac:dyDescent="0.3">
@@ -5223,19 +5224,19 @@
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="0"/>
-        <v>2.65</v>
+        <v>3.89</v>
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="2"/>
-        <v>4.8250000000000002</v>
+        <v>5.4450000000000003</v>
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.37010159651669094</v>
+        <v>0.9772727272727274</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.39035746742197186</v>
+        <v>0.2181665254695902</v>
       </c>
     </row>
     <row r="26" spans="3:12" x14ac:dyDescent="0.3">
@@ -5247,19 +5248,19 @@
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="0"/>
-        <v>4.49</v>
+        <v>3.07</v>
       </c>
       <c r="F26">
         <f t="shared" ca="1" si="2"/>
-        <v>5.7450000000000001</v>
+        <v>5.0350000000000001</v>
       </c>
       <c r="G26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.6371552975326561</v>
+        <v>0.80785123966942152</v>
       </c>
       <c r="H26">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.18672811494854619</v>
+        <v>0.49350835455313907</v>
       </c>
     </row>
     <row r="27" spans="3:12" x14ac:dyDescent="0.3">
@@ -5271,19 +5272,19 @@
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>3.98</v>
       </c>
       <c r="F27">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>5.49</v>
       </c>
       <c r="G27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.42089985486211901</v>
+        <v>0.99586776859504145</v>
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.12127796780747488</v>
+        <v>0.7410919198822381</v>
       </c>
     </row>
     <row r="28" spans="3:12" x14ac:dyDescent="0.3">
@@ -5295,19 +5296,19 @@
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.6399999999999997</v>
+        <v>4</v>
       </c>
       <c r="F28">
         <f t="shared" ca="1" si="2"/>
-        <v>5.82</v>
+        <v>5.5</v>
       </c>
       <c r="G28">
         <f t="shared" ca="1" si="1"/>
-        <v>0.65892597968069677</v>
+        <v>1</v>
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="3"/>
-        <v>4.2726795823512506E-2</v>
+        <v>0.99051379849270349</v>
       </c>
     </row>
     <row r="29" spans="3:12" x14ac:dyDescent="0.3">
@@ -5319,19 +5320,19 @@
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5</v>
+        <v>3.54</v>
       </c>
       <c r="F29">
         <f t="shared" ca="1" si="2"/>
-        <v>4.75</v>
+        <v>5.27</v>
       </c>
       <c r="G29">
         <f t="shared" ca="1" si="1"/>
-        <v>0.34833091436865021</v>
+        <v>0.90495867768595029</v>
       </c>
       <c r="H29">
         <f t="shared" ca="1" si="3"/>
-        <v>5.8670411735280086E-2</v>
+        <v>0.77314666355519157</v>
       </c>
     </row>
     <row r="30" spans="3:12" x14ac:dyDescent="0.3">
@@ -5343,19 +5344,19 @@
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="0"/>
-        <v>5.69</v>
+        <v>3.9</v>
       </c>
       <c r="F30">
         <f t="shared" ca="1" si="2"/>
-        <v>6.3450000000000006</v>
+        <v>5.45</v>
       </c>
       <c r="G30">
         <f t="shared" ca="1" si="1"/>
-        <v>0.81132075471698128</v>
+        <v>0.97933884297520668</v>
       </c>
       <c r="H30">
         <f t="shared" ca="1" si="3"/>
-        <v>7.1432691801798578E-2</v>
+        <v>0.4838390338424548</v>
       </c>
     </row>
     <row r="31" spans="3:12" x14ac:dyDescent="0.3">
@@ -5367,19 +5368,19 @@
       </c>
       <c r="E31">
         <f t="shared" ca="1" si="0"/>
-        <v>6.48</v>
+        <v>3.97</v>
       </c>
       <c r="F31">
         <f t="shared" ca="1" si="2"/>
-        <v>6.74</v>
+        <v>5.4850000000000003</v>
       </c>
       <c r="G31">
         <f t="shared" ca="1" si="1"/>
-        <v>0.92597968069666181</v>
+        <v>0.99380165289256217</v>
       </c>
       <c r="H31">
         <f t="shared" ca="1" si="3"/>
-        <v>1.1014666069011244E-2</v>
+        <v>0.26960441114580841</v>
       </c>
     </row>
     <row r="32" spans="3:12" x14ac:dyDescent="0.3">
@@ -5391,19 +5392,19 @@
       </c>
       <c r="E32">
         <f t="shared" ca="1" si="0"/>
-        <v>6.56</v>
+        <v>3.71</v>
       </c>
       <c r="F32">
         <f t="shared" ca="1" si="2"/>
-        <v>6.7799999999999994</v>
+        <v>5.3550000000000004</v>
       </c>
       <c r="G32">
         <f t="shared" ca="1" si="1"/>
-        <v>0.93759071117561665</v>
+        <v>0.94008264462809932</v>
       </c>
       <c r="H32">
         <f t="shared" ca="1" si="3"/>
-        <v>0.11504147647164607</v>
+        <v>-5.0186971546129821E-3</v>
       </c>
     </row>
     <row r="33" spans="3:8" x14ac:dyDescent="0.3">
@@ -5415,19 +5416,19 @@
       </c>
       <c r="E33">
         <f t="shared" ca="1" si="0"/>
-        <v>6.87</v>
+        <v>3.72</v>
       </c>
       <c r="F33">
         <f t="shared" ca="1" si="2"/>
-        <v>6.9350000000000005</v>
+        <v>5.36</v>
       </c>
       <c r="G33">
         <f t="shared" ca="1" si="1"/>
-        <v>0.98258345428156757</v>
+        <v>0.94214876033057859</v>
       </c>
       <c r="H33">
         <f t="shared" ca="1" si="3"/>
-        <v>6.6472456379569236E-2</v>
+        <v>-0.25642581948010973</v>
       </c>
     </row>
     <row r="34" spans="3:8" x14ac:dyDescent="0.3">
@@ -5435,23 +5436,23 @@
         <v>1.5</v>
       </c>
       <c r="D34">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E34">
         <f t="shared" ca="1" si="0"/>
-        <v>3.78</v>
+        <v>3.67</v>
       </c>
       <c r="F34">
         <f t="shared" ca="1" si="2"/>
-        <v>5.39</v>
+        <v>3.335</v>
       </c>
       <c r="G34">
         <f t="shared" ca="1" si="1"/>
-        <v>0.5341074020319303</v>
+        <v>0.10537190082644624</v>
       </c>
       <c r="H34">
         <f t="shared" ca="1" si="3"/>
-        <v>0.10652405228776121</v>
+        <v>-0.4828862704247891</v>
       </c>
     </row>
     <row r="35" spans="3:8" x14ac:dyDescent="0.3">
@@ -5459,23 +5460,23 @@
         <v>1.55</v>
       </c>
       <c r="D35">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E35">
         <f t="shared" ca="1" si="0"/>
-        <v>6.83</v>
+        <v>3.16</v>
       </c>
       <c r="F35">
         <f t="shared" ca="1" si="2"/>
-        <v>6.915</v>
+        <v>3.08</v>
       </c>
       <c r="G35">
         <f t="shared" ca="1" si="1"/>
-        <v>0.97677793904208998</v>
+        <v>0</v>
       </c>
       <c r="H35">
         <f t="shared" ca="1" si="3"/>
-        <v>0.14937962817293723</v>
+        <v>-0.43191253808407526</v>
       </c>
     </row>
     <row r="36" spans="3:8" x14ac:dyDescent="0.3">
@@ -5483,23 +5484,23 @@
         <v>1.6</v>
       </c>
       <c r="D36">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E36">
         <f t="shared" ref="E36:E67" ca="1" si="4">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>2.21</v>
+        <v>3.96</v>
       </c>
       <c r="F36">
         <f t="shared" ca="1" si="2"/>
-        <v>4.6050000000000004</v>
+        <v>3.48</v>
       </c>
       <c r="G36">
         <f t="shared" ref="G36:G67" ca="1" si="5">(F36-minval)/(maxval-minval)</f>
-        <v>0.30624092888243848</v>
+        <v>0.16528925619834708</v>
       </c>
       <c r="H36">
         <f t="shared" ca="1" si="3"/>
-        <v>0.40649326652375867</v>
+        <v>-0.33672075738205337</v>
       </c>
     </row>
     <row r="37" spans="3:8" x14ac:dyDescent="0.3">
@@ -5507,23 +5508,23 @@
         <v>1.65</v>
       </c>
       <c r="D37">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E37">
         <f t="shared" ca="1" si="4"/>
-        <v>3.25</v>
+        <v>3.3</v>
       </c>
       <c r="F37">
         <f t="shared" ca="1" si="2"/>
-        <v>5.125</v>
+        <v>3.15</v>
       </c>
       <c r="G37">
         <f t="shared" ca="1" si="5"/>
-        <v>0.45718432510885343</v>
+        <v>2.8925619834710679E-2</v>
       </c>
       <c r="H37">
         <f t="shared" ca="1" si="3"/>
-        <v>0.23108013365793517</v>
+        <v>-0.31466327287112095</v>
       </c>
     </row>
     <row r="38" spans="3:8" x14ac:dyDescent="0.3">
@@ -5531,23 +5532,23 @@
         <v>1.7</v>
       </c>
       <c r="D38">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E38">
         <f t="shared" ca="1" si="4"/>
-        <v>5.97</v>
+        <v>3.6</v>
       </c>
       <c r="F38">
         <f t="shared" ca="1" si="2"/>
-        <v>6.4849999999999994</v>
+        <v>3.3</v>
       </c>
       <c r="G38">
         <f t="shared" ca="1" si="5"/>
-        <v>0.85195936139332351</v>
+        <v>9.0909090909090814E-2</v>
       </c>
       <c r="H38">
         <f t="shared" ca="1" si="3"/>
-        <v>0.12796207163768505</v>
+        <v>-0.26425442241738445</v>
       </c>
     </row>
     <row r="39" spans="3:8" x14ac:dyDescent="0.3">
@@ -5555,23 +5556,23 @@
         <v>1.75</v>
       </c>
       <c r="D39">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E39">
         <f t="shared" ca="1" si="4"/>
-        <v>4.5</v>
+        <v>3.42</v>
       </c>
       <c r="F39">
         <f t="shared" ca="1" si="2"/>
-        <v>5.75</v>
+        <v>3.21</v>
       </c>
       <c r="G39">
         <f t="shared" ca="1" si="5"/>
-        <v>0.63860667634252544</v>
+        <v>5.371900826446277E-2</v>
       </c>
       <c r="H39">
         <f t="shared" ca="1" si="3"/>
-        <v>0.22817358826099599</v>
+        <v>-0.13832789870435269</v>
       </c>
     </row>
     <row r="40" spans="3:8" x14ac:dyDescent="0.3">
@@ -5583,19 +5584,19 @@
       </c>
       <c r="E40">
         <f t="shared" ca="1" si="4"/>
-        <v>3.04</v>
+        <v>3.3</v>
       </c>
       <c r="F40">
         <f t="shared" ca="1" si="2"/>
-        <v>5.0199999999999996</v>
+        <v>5.15</v>
       </c>
       <c r="G40">
         <f t="shared" ca="1" si="5"/>
-        <v>0.42670537010159643</v>
+        <v>0.85537190082644643</v>
       </c>
       <c r="H40">
         <f t="shared" ca="1" si="3"/>
-        <v>7.0912332040516182E-2</v>
+        <v>-0.1431499632721327</v>
       </c>
     </row>
     <row r="41" spans="3:8" x14ac:dyDescent="0.3">
@@ -5607,19 +5608,19 @@
       </c>
       <c r="E41">
         <f t="shared" ca="1" si="4"/>
-        <v>6.41</v>
+        <v>3.96</v>
       </c>
       <c r="F41">
         <f t="shared" ca="1" si="2"/>
-        <v>6.7050000000000001</v>
+        <v>5.48</v>
       </c>
       <c r="G41">
         <f t="shared" ca="1" si="5"/>
-        <v>0.9158200290275762</v>
+        <v>0.99173553719008278</v>
       </c>
       <c r="H41">
         <f t="shared" ca="1" si="3"/>
-        <v>-8.9379456812388666E-2</v>
+        <v>-0.20843954033548764</v>
       </c>
     </row>
     <row r="42" spans="3:8" x14ac:dyDescent="0.3">
@@ -5631,19 +5632,19 @@
       </c>
       <c r="E42">
         <f t="shared" ca="1" si="4"/>
-        <v>3.25</v>
+        <v>3.51</v>
       </c>
       <c r="F42">
         <f t="shared" ca="1" si="2"/>
-        <v>5.125</v>
+        <v>5.2549999999999999</v>
       </c>
       <c r="G42">
         <f t="shared" ca="1" si="5"/>
-        <v>0.45718432510885343</v>
+        <v>0.89876033057851235</v>
       </c>
       <c r="H42">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.36588865003538718</v>
+        <v>-0.36663040301010086</v>
       </c>
     </row>
     <row r="43" spans="3:8" x14ac:dyDescent="0.3">
@@ -5655,19 +5656,19 @@
       </c>
       <c r="E43">
         <f t="shared" ca="1" si="4"/>
-        <v>0.2</v>
+        <v>3.86</v>
       </c>
       <c r="F43">
         <f t="shared" ca="1" si="2"/>
-        <v>3.6</v>
+        <v>5.43</v>
       </c>
       <c r="G43">
         <f t="shared" ca="1" si="5"/>
-        <v>1.4513788098693836E-2</v>
+        <v>0.97107438016528913</v>
       </c>
       <c r="H43">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.16205311927206142</v>
+        <v>-3.976526620841471E-2</v>
       </c>
     </row>
     <row r="44" spans="3:8" x14ac:dyDescent="0.3">
@@ -5679,19 +5680,19 @@
       </c>
       <c r="E44">
         <f t="shared" ca="1" si="4"/>
-        <v>5.74</v>
+        <v>3.59</v>
       </c>
       <c r="F44">
         <f t="shared" ca="1" si="2"/>
-        <v>6.37</v>
+        <v>5.2949999999999999</v>
       </c>
       <c r="G44">
         <f t="shared" ca="1" si="5"/>
-        <v>0.81857764876632799</v>
+        <v>0.91528925619834711</v>
       </c>
       <c r="H44">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.32073912181138986</v>
+        <v>0.18922361658111589</v>
       </c>
     </row>
     <row r="45" spans="3:8" x14ac:dyDescent="0.3">
@@ -5703,19 +5704,19 @@
       </c>
       <c r="E45">
         <f t="shared" ca="1" si="4"/>
-        <v>3.72</v>
+        <v>3.07</v>
       </c>
       <c r="F45">
         <f t="shared" ca="1" si="2"/>
-        <v>5.36</v>
+        <v>5.0350000000000001</v>
       </c>
       <c r="G45">
         <f t="shared" ca="1" si="5"/>
-        <v>0.52539912917271414</v>
+        <v>0.80785123966942152</v>
       </c>
       <c r="H45">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.31432674138231625</v>
+        <v>-3.9801889730957433E-2</v>
       </c>
     </row>
     <row r="46" spans="3:8" x14ac:dyDescent="0.3">
@@ -5727,19 +5728,19 @@
       </c>
       <c r="E46">
         <f t="shared" ca="1" si="4"/>
-        <v>3.21</v>
+        <v>3.6</v>
       </c>
       <c r="F46">
         <f t="shared" ca="1" si="2"/>
-        <v>5.1050000000000004</v>
+        <v>5.3</v>
       </c>
       <c r="G46">
         <f t="shared" ca="1" si="5"/>
-        <v>0.45137880986937606</v>
+        <v>0.91735537190082639</v>
       </c>
       <c r="H46">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.16046111942342989</v>
+        <v>8.2127981537410591E-2</v>
       </c>
     </row>
     <row r="47" spans="3:8" x14ac:dyDescent="0.3">
@@ -5751,19 +5752,19 @@
       </c>
       <c r="E47">
         <f t="shared" ca="1" si="4"/>
-        <v>1.92</v>
+        <v>3.45</v>
       </c>
       <c r="F47">
         <f t="shared" ca="1" si="2"/>
-        <v>4.46</v>
+        <v>5.2249999999999996</v>
       </c>
       <c r="G47">
         <f t="shared" ca="1" si="5"/>
-        <v>0.26415094339622641</v>
+        <v>0.88636363636363624</v>
       </c>
       <c r="H47">
         <f t="shared" ca="1" si="3"/>
-        <v>-5.7828124243944859E-2</v>
+        <v>0.13501497426859002</v>
       </c>
     </row>
     <row r="48" spans="3:8" x14ac:dyDescent="0.3">
@@ -5775,19 +5776,19 @@
       </c>
       <c r="E48">
         <f t="shared" ca="1" si="4"/>
-        <v>5.86</v>
+        <v>3.85</v>
       </c>
       <c r="F48">
         <f t="shared" ca="1" si="2"/>
-        <v>6.43</v>
+        <v>5.4249999999999998</v>
       </c>
       <c r="G48">
         <f t="shared" ca="1" si="5"/>
-        <v>0.83599419448476042</v>
+        <v>0.96900826446280985</v>
       </c>
       <c r="H48">
         <f t="shared" ca="1" si="3"/>
-        <v>0.18660134279130239</v>
+        <v>0.29489844238856366</v>
       </c>
     </row>
     <row r="49" spans="3:8" x14ac:dyDescent="0.3">
@@ -5799,19 +5800,19 @@
       </c>
       <c r="E49">
         <f t="shared" ca="1" si="4"/>
-        <v>2.39</v>
+        <v>3.97</v>
       </c>
       <c r="F49">
         <f t="shared" ca="1" si="2"/>
-        <v>4.6950000000000003</v>
+        <v>5.4850000000000003</v>
       </c>
       <c r="G49">
         <f t="shared" ca="1" si="5"/>
-        <v>0.33236574746008718</v>
+        <v>0.99380165289256217</v>
       </c>
       <c r="H49">
         <f t="shared" ca="1" si="3"/>
-        <v>0.18288590935742746</v>
+        <v>0.19878183280675699</v>
       </c>
     </row>
     <row r="50" spans="3:8" x14ac:dyDescent="0.3">
@@ -5823,19 +5824,19 @@
       </c>
       <c r="E50">
         <f t="shared" ca="1" si="4"/>
-        <v>3.37</v>
+        <v>3.26</v>
       </c>
       <c r="F50">
         <f t="shared" ca="1" si="2"/>
-        <v>5.1850000000000005</v>
+        <v>5.13</v>
       </c>
       <c r="G50">
         <f t="shared" ca="1" si="5"/>
-        <v>0.47460087082728608</v>
+        <v>0.84710743801652888</v>
       </c>
       <c r="H50">
         <f t="shared" ca="1" si="3"/>
-        <v>0.4615481532140136</v>
+        <v>-3.9736745314926096E-2</v>
       </c>
     </row>
     <row r="51" spans="3:8" x14ac:dyDescent="0.3">
@@ -5847,19 +5848,19 @@
       </c>
       <c r="E51">
         <f t="shared" ca="1" si="4"/>
-        <v>6.27</v>
+        <v>3.56</v>
       </c>
       <c r="F51">
         <f t="shared" ca="1" si="2"/>
-        <v>6.6349999999999998</v>
+        <v>5.28</v>
       </c>
       <c r="G51">
         <f t="shared" ca="1" si="5"/>
-        <v>0.89550072568940486</v>
+        <v>0.90909090909090917</v>
       </c>
       <c r="H51">
         <f t="shared" ca="1" si="3"/>
-        <v>0.35869732019948442</v>
+        <v>-2.998773752251637E-3</v>
       </c>
     </row>
     <row r="52" spans="3:8" x14ac:dyDescent="0.3">
@@ -5871,19 +5872,19 @@
       </c>
       <c r="E52">
         <f t="shared" ca="1" si="4"/>
-        <v>6.6</v>
+        <v>3.86</v>
       </c>
       <c r="F52">
         <f t="shared" ca="1" si="2"/>
-        <v>6.8</v>
+        <v>5.43</v>
       </c>
       <c r="G52">
         <f t="shared" ca="1" si="5"/>
-        <v>0.94339622641509424</v>
+        <v>0.97107438016528913</v>
       </c>
       <c r="H52">
         <f t="shared" ca="1" si="3"/>
-        <v>0.26196042006903419</v>
+        <v>4.438442905181886E-3</v>
       </c>
     </row>
     <row r="53" spans="3:8" x14ac:dyDescent="0.3">
@@ -5895,19 +5896,19 @@
       </c>
       <c r="E53">
         <f t="shared" ca="1" si="4"/>
-        <v>4.51</v>
+        <v>3.58</v>
       </c>
       <c r="F53">
         <f t="shared" ca="1" si="2"/>
-        <v>5.7549999999999999</v>
+        <v>5.29</v>
       </c>
       <c r="G53">
         <f t="shared" ca="1" si="5"/>
-        <v>0.64005805515239478</v>
+        <v>0.91322314049586784</v>
       </c>
       <c r="H53">
         <f t="shared" ca="1" si="3"/>
-        <v>0.12467132923633227</v>
+        <v>8.7680642090914182E-2</v>
       </c>
     </row>
     <row r="54" spans="3:8" x14ac:dyDescent="0.3">
@@ -5919,19 +5920,19 @@
       </c>
       <c r="E54">
         <f t="shared" ca="1" si="4"/>
-        <v>2.16</v>
+        <v>3.02</v>
       </c>
       <c r="F54">
         <f t="shared" ca="1" si="2"/>
-        <v>4.58</v>
+        <v>5.01</v>
       </c>
       <c r="G54">
         <f t="shared" ca="1" si="5"/>
-        <v>0.29898403483309149</v>
+        <v>0.79752066115702469</v>
       </c>
       <c r="H54">
         <f t="shared" ca="1" si="3"/>
-        <v>-4.1250886435076066E-2</v>
+        <v>-0.21243195293665049</v>
       </c>
     </row>
     <row r="55" spans="3:8" x14ac:dyDescent="0.3">
@@ -5943,19 +5944,19 @@
       </c>
       <c r="E55">
         <f t="shared" ca="1" si="4"/>
-        <v>5.2</v>
+        <v>3.39</v>
       </c>
       <c r="F55">
         <f t="shared" ca="1" si="2"/>
-        <v>6.1</v>
+        <v>5.1950000000000003</v>
       </c>
       <c r="G55">
         <f t="shared" ca="1" si="5"/>
-        <v>0.74020319303338156</v>
+        <v>0.87396694214876047</v>
       </c>
       <c r="H55">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.14903892383910067</v>
+        <v>-0.44962377747724597</v>
       </c>
     </row>
     <row r="56" spans="3:8" x14ac:dyDescent="0.3">
@@ -5967,19 +5968,19 @@
       </c>
       <c r="E56">
         <f t="shared" ca="1" si="4"/>
-        <v>3.14</v>
+        <v>3.86</v>
       </c>
       <c r="F56">
         <f t="shared" ca="1" si="2"/>
-        <v>5.07</v>
+        <v>5.43</v>
       </c>
       <c r="G56">
         <f t="shared" ca="1" si="5"/>
-        <v>0.4412191582002904</v>
+        <v>0.97107438016528913</v>
       </c>
       <c r="H56">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.42752420639518218</v>
+        <v>-0.17238356497697213</v>
       </c>
     </row>
     <row r="57" spans="3:8" x14ac:dyDescent="0.3">
@@ -5991,19 +5992,19 @@
       </c>
       <c r="E57">
         <f t="shared" ca="1" si="4"/>
-        <v>5.24</v>
+        <v>3.34</v>
       </c>
       <c r="F57">
         <f t="shared" ca="1" si="2"/>
-        <v>6.12</v>
+        <v>5.17</v>
       </c>
       <c r="G57">
         <f t="shared" ca="1" si="5"/>
-        <v>0.74600870827285926</v>
+        <v>0.86363636363636365</v>
       </c>
       <c r="H57">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.43870683637437841</v>
+        <v>-1.8441523356356973E-3</v>
       </c>
     </row>
     <row r="58" spans="3:8" x14ac:dyDescent="0.3">
@@ -6015,19 +6016,19 @@
       </c>
       <c r="E58">
         <f t="shared" ca="1" si="4"/>
-        <v>5.96</v>
+        <v>3.64</v>
       </c>
       <c r="F58">
         <f t="shared" ca="1" si="2"/>
-        <v>6.48</v>
+        <v>5.32</v>
       </c>
       <c r="G58">
         <f t="shared" ca="1" si="5"/>
-        <v>0.85050798258345439</v>
+        <v>0.92561983471074394</v>
       </c>
       <c r="H58">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.47791162805923354</v>
+        <v>-1.5367497398268893E-2</v>
       </c>
     </row>
     <row r="59" spans="3:8" x14ac:dyDescent="0.3">
@@ -6039,19 +6040,19 @@
       </c>
       <c r="E59">
         <f t="shared" ca="1" si="4"/>
-        <v>1.29</v>
+        <v>3.33</v>
       </c>
       <c r="F59">
         <f t="shared" ca="1" si="2"/>
-        <v>4.1449999999999996</v>
+        <v>5.165</v>
       </c>
       <c r="G59">
         <f t="shared" ca="1" si="5"/>
-        <v>0.17271407837445565</v>
+        <v>0.86157024793388426</v>
       </c>
       <c r="H59">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.24802126068435185</v>
+        <v>-0.10439088410218882</v>
       </c>
     </row>
     <row r="60" spans="3:8" x14ac:dyDescent="0.3">
@@ -6063,19 +6064,19 @@
       </c>
       <c r="E60">
         <f t="shared" ca="1" si="4"/>
-        <v>1.2</v>
+        <v>3.24</v>
       </c>
       <c r="F60">
         <f t="shared" ca="1" si="2"/>
-        <v>4.0999999999999996</v>
+        <v>5.12</v>
       </c>
       <c r="G60">
         <f t="shared" ca="1" si="5"/>
-        <v>0.15965166908563128</v>
+        <v>0.84297520661157033</v>
       </c>
       <c r="H60">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.19392000361721173</v>
+        <v>0.29081624250727883</v>
       </c>
     </row>
     <row r="61" spans="3:8" x14ac:dyDescent="0.3">
@@ -6087,19 +6088,19 @@
       </c>
       <c r="E61">
         <f t="shared" ca="1" si="4"/>
-        <v>2.15</v>
+        <v>3.69</v>
       </c>
       <c r="F61">
         <f t="shared" ca="1" si="2"/>
-        <v>4.5750000000000002</v>
+        <v>5.3449999999999998</v>
       </c>
       <c r="G61">
         <f t="shared" ca="1" si="5"/>
-        <v>0.29753265602322215</v>
+        <v>0.93595041322314043</v>
       </c>
       <c r="H61">
         <f t="shared" ca="1" si="3"/>
-        <v>-2.2671070106898884E-2</v>
+        <v>0.59175091331526297</v>
       </c>
     </row>
     <row r="62" spans="3:8" x14ac:dyDescent="0.3">
@@ -6111,19 +6112,19 @@
       </c>
       <c r="E62">
         <f t="shared" ca="1" si="4"/>
-        <v>5.46</v>
+        <v>3.82</v>
       </c>
       <c r="F62">
         <f t="shared" ca="1" si="2"/>
-        <v>6.23</v>
+        <v>5.41</v>
       </c>
       <c r="G62">
         <f t="shared" ca="1" si="5"/>
-        <v>0.77793904208998554</v>
+        <v>0.96280991735537191</v>
       </c>
       <c r="H62">
         <f t="shared" ca="1" si="3"/>
-        <v>0.19400286329330171</v>
+        <v>0.32463061034782065</v>
       </c>
     </row>
     <row r="63" spans="3:8" x14ac:dyDescent="0.3">
@@ -6135,19 +6136,19 @@
       </c>
       <c r="E63">
         <f t="shared" ca="1" si="4"/>
-        <v>6.93</v>
+        <v>3.24</v>
       </c>
       <c r="F63">
         <f t="shared" ca="1" si="2"/>
-        <v>6.9649999999999999</v>
+        <v>5.12</v>
       </c>
       <c r="G63">
         <f t="shared" ca="1" si="5"/>
-        <v>0.99129172714078362</v>
+        <v>0.84297520661157033</v>
       </c>
       <c r="H63">
         <f t="shared" ca="1" si="3"/>
-        <v>0.5218867347813364</v>
+        <v>9.5749083177827751E-2</v>
       </c>
     </row>
     <row r="64" spans="3:8" x14ac:dyDescent="0.3">
@@ -6159,19 +6160,19 @@
       </c>
       <c r="E64">
         <f t="shared" ca="1" si="4"/>
-        <v>6.14</v>
+        <v>3.31</v>
       </c>
       <c r="F64">
         <f t="shared" ca="1" si="2"/>
-        <v>6.57</v>
+        <v>5.1550000000000002</v>
       </c>
       <c r="G64">
         <f t="shared" ca="1" si="5"/>
-        <v>0.87663280116110309</v>
+        <v>0.85743801652892571</v>
       </c>
       <c r="H64">
         <f t="shared" ca="1" si="3"/>
-        <v>0.71289966635871693</v>
+        <v>6.5516611112358916E-2</v>
       </c>
     </row>
     <row r="65" spans="3:8" x14ac:dyDescent="0.3">
@@ -6183,19 +6184,19 @@
       </c>
       <c r="E65">
         <f t="shared" ca="1" si="4"/>
-        <v>3.89</v>
+        <v>3.87</v>
       </c>
       <c r="F65">
         <f t="shared" ca="1" si="2"/>
-        <v>5.4450000000000003</v>
+        <v>5.4350000000000005</v>
       </c>
       <c r="G65">
         <f t="shared" ca="1" si="5"/>
-        <v>0.55007256894049361</v>
+        <v>0.97314049586776885</v>
       </c>
       <c r="H65">
         <f t="shared" ca="1" si="3"/>
-        <v>0.45158903053802463</v>
+        <v>6.5710329107352861E-2</v>
       </c>
     </row>
     <row r="66" spans="3:8" x14ac:dyDescent="0.3">
@@ -6207,19 +6208,19 @@
       </c>
       <c r="E66">
         <f t="shared" ca="1" si="4"/>
-        <v>2.77</v>
+        <v>3.82</v>
       </c>
       <c r="F66">
         <f t="shared" ca="1" si="2"/>
-        <v>4.8849999999999998</v>
+        <v>5.41</v>
       </c>
       <c r="G66">
         <f t="shared" ca="1" si="5"/>
-        <v>0.38751814223512332</v>
+        <v>0.96280991735537191</v>
       </c>
       <c r="H66">
         <f t="shared" ca="1" si="3"/>
-        <v>0.49403166197486664</v>
+        <v>-0.36760226344226715</v>
       </c>
     </row>
     <row r="67" spans="3:8" x14ac:dyDescent="0.3">
@@ -6231,19 +6232,19 @@
       </c>
       <c r="E67">
         <f t="shared" ca="1" si="4"/>
-        <v>6.89</v>
+        <v>3.2</v>
       </c>
       <c r="F67">
         <f t="shared" ca="1" si="2"/>
-        <v>6.9450000000000003</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="G67">
         <f t="shared" ca="1" si="5"/>
-        <v>0.98548621190130625</v>
+        <v>0.83471074380165278</v>
       </c>
       <c r="H67">
         <f t="shared" ca="1" si="3"/>
-        <v>0.30377090123173667</v>
+        <v>-0.75191000825309684</v>
       </c>
     </row>
     <row r="68" spans="3:8" x14ac:dyDescent="0.3">
@@ -6255,19 +6256,19 @@
       </c>
       <c r="E68">
         <f t="shared" ref="E68:E74" ca="1" si="6">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>5.32</v>
+        <v>3.39</v>
       </c>
       <c r="F68">
         <f t="shared" ca="1" si="2"/>
-        <v>6.16</v>
+        <v>5.1950000000000003</v>
       </c>
       <c r="G68">
-        <f t="shared" ref="G68:G99" ca="1" si="7">(F68-minval)/(maxval-minval)</f>
-        <v>0.75761973875181421</v>
+        <f t="shared" ref="G68:G74" ca="1" si="7">(F68-minval)/(maxval-minval)</f>
+        <v>0.87396694214876047</v>
       </c>
       <c r="H68">
         <f t="shared" ca="1" si="3"/>
-        <v>0.51644899900445196</v>
+        <v>-0.55109859209697132</v>
       </c>
     </row>
     <row r="69" spans="3:8" x14ac:dyDescent="0.3">
@@ -6279,15 +6280,15 @@
       </c>
       <c r="E69">
         <f t="shared" ca="1" si="6"/>
-        <v>6.99</v>
+        <v>3.31</v>
       </c>
       <c r="F69">
         <f t="shared" ref="F69:F74" ca="1" si="8">(D69+E69)/2</f>
-        <v>6.9950000000000001</v>
+        <v>5.1550000000000002</v>
       </c>
       <c r="G69">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>0.85743801652892571</v>
       </c>
     </row>
     <row r="70" spans="3:8" x14ac:dyDescent="0.3">
@@ -6299,15 +6300,15 @@
       </c>
       <c r="E70">
         <f t="shared" ca="1" si="6"/>
-        <v>0.76</v>
+        <v>3.4</v>
       </c>
       <c r="F70">
         <f t="shared" ca="1" si="8"/>
-        <v>3.88</v>
+        <v>5.2</v>
       </c>
       <c r="G70">
         <f t="shared" ca="1" si="7"/>
-        <v>9.5791001451378824E-2</v>
+        <v>0.87603305785123975</v>
       </c>
     </row>
     <row r="71" spans="3:8" x14ac:dyDescent="0.3">
@@ -6319,15 +6320,15 @@
       </c>
       <c r="E71">
         <f t="shared" ca="1" si="6"/>
-        <v>3.67</v>
+        <v>3.27</v>
       </c>
       <c r="F71">
         <f t="shared" ca="1" si="8"/>
-        <v>5.335</v>
+        <v>5.1349999999999998</v>
       </c>
       <c r="G71">
         <f t="shared" ca="1" si="7"/>
-        <v>0.51814223512336721</v>
+        <v>0.84917355371900816</v>
       </c>
     </row>
     <row r="72" spans="3:8" x14ac:dyDescent="0.3">
@@ -6339,15 +6340,15 @@
       </c>
       <c r="E72">
         <f t="shared" ca="1" si="6"/>
-        <v>0.93</v>
+        <v>3.49</v>
       </c>
       <c r="F72">
         <f t="shared" ca="1" si="8"/>
-        <v>3.9649999999999999</v>
+        <v>5.2450000000000001</v>
       </c>
       <c r="G72">
         <f t="shared" ca="1" si="7"/>
-        <v>0.1204644412191582</v>
+        <v>0.89462809917355379</v>
       </c>
     </row>
     <row r="73" spans="3:8" x14ac:dyDescent="0.3">
@@ -6359,15 +6360,15 @@
       </c>
       <c r="E73">
         <f t="shared" ca="1" si="6"/>
-        <v>4.46</v>
+        <v>3.55</v>
       </c>
       <c r="F73">
         <f t="shared" ca="1" si="8"/>
-        <v>5.73</v>
+        <v>5.2750000000000004</v>
       </c>
       <c r="G73">
         <f t="shared" ca="1" si="7"/>
-        <v>0.63280116110304807</v>
+        <v>0.9070247933884299</v>
       </c>
     </row>
     <row r="74" spans="3:8" x14ac:dyDescent="0.3">
@@ -6379,15 +6380,15 @@
       </c>
       <c r="E74">
         <f t="shared" ca="1" si="6"/>
-        <v>0.1</v>
+        <v>3.57</v>
       </c>
       <c r="F74">
         <f t="shared" ca="1" si="8"/>
-        <v>3.55</v>
+        <v>5.2850000000000001</v>
       </c>
       <c r="G74">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>0.91115702479338845</v>
       </c>
     </row>
   </sheetData>

</xml_diff>